<commit_message>
update (included exmple vox file)
</commit_message>
<xml_diff>
--- a/Dream3d2Abaqus/inputfile_info.xlsx
+++ b/Dream3d2Abaqus/inputfile_info.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mi19356\OneDrive - University of Bristol\MATLAB\316H_input\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mi19356\OneDrive - University of Bristol\Documents\CP_simulations\Dream3d2Abaqus\Dream3d2Abaqus\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="6" documentId="8_{B136ABAE-EB51-4A80-BA81-9E123800CD73}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{CD4DF392-C7EF-4A2B-BFE8-9592B8A7D985}"/>
+  <xr:revisionPtr revIDLastSave="16" documentId="8_{B136ABAE-EB51-4A80-BA81-9E123800CD73}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{DD30ADD4-E938-434D-98EA-BC9D9461AF90}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="1" xr2:uid="{B2FFBA9E-8DF3-44DC-8BFA-5D5291E16B1C}"/>
+    <workbookView xWindow="380" yWindow="380" windowWidth="13880" windowHeight="9190" xr2:uid="{B2FFBA9E-8DF3-44DC-8BFA-5D5291E16B1C}"/>
   </bookViews>
   <sheets>
     <sheet name="Material_parameters" sheetId="1" r:id="rId1"/>
@@ -382,25 +382,25 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0A2FF6DC-890B-49C6-8880-6BB58835CE0B}">
   <dimension ref="A1:A168"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:A168"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A166" sqref="A166"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A1">
-        <v>157000</v>
+        <v>183900</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A2">
-        <v>102500</v>
+        <v>123400</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A3">
-        <v>101000</v>
+        <v>91500</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.35">
@@ -750,7 +750,7 @@
     </row>
     <row r="73" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A73">
-        <v>80</v>
+        <v>500</v>
       </c>
     </row>
     <row r="74" spans="1:1" x14ac:dyDescent="0.35">
@@ -1165,7 +1165,7 @@
     </row>
     <row r="156" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A156">
-        <v>0.245</v>
+        <v>0.35</v>
       </c>
     </row>
     <row r="157" spans="1:1" x14ac:dyDescent="0.35">
@@ -1195,7 +1195,7 @@
     </row>
     <row r="162" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A162">
-        <v>700</v>
+        <v>245</v>
       </c>
     </row>
     <row r="163" spans="1:1" x14ac:dyDescent="0.35">
@@ -1210,7 +1210,7 @@
     </row>
     <row r="165" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A165">
-        <v>10000</v>
+        <v>6555</v>
       </c>
     </row>
     <row r="166" spans="1:1" x14ac:dyDescent="0.35">
@@ -1238,2804 +1238,2804 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C8E9C165-EF39-4A1B-9ECE-A782E2B0DD1A}">
   <dimension ref="A1:C254"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A246" workbookViewId="0">
-      <selection activeCell="A255" sqref="A255:C302"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:C254"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A1">
-        <v>13.105769</v>
+        <v>9.0500001999999995</v>
       </c>
       <c r="B1">
-        <v>6.7115383</v>
+        <v>3.6500001000000002</v>
       </c>
       <c r="C1">
-        <v>11.932693</v>
+        <v>1.8571428000000001</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A2">
-        <v>7.0290698999999996</v>
+        <v>3.8646498</v>
       </c>
       <c r="B2">
-        <v>12.746124</v>
+        <v>1.7277070000000001</v>
       </c>
       <c r="C2">
-        <v>7.8275193999999999</v>
+        <v>5.9570065000000003</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A3">
-        <v>13.544117999999999</v>
+        <v>7.75</v>
       </c>
       <c r="B3">
-        <v>7.7205881999999999</v>
+        <v>10.75</v>
       </c>
       <c r="C3">
-        <v>6.4264707999999997</v>
+        <v>0.75</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A4">
-        <v>0.93253969999999997</v>
+        <v>5.6829267000000003</v>
       </c>
       <c r="B4">
-        <v>8.5198412000000001</v>
+        <v>8.8414631000000004</v>
       </c>
       <c r="C4">
-        <v>4.9801587999999999</v>
+        <v>4.9268292999999996</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A5">
-        <v>10.587210000000001</v>
+        <v>3.8622448</v>
       </c>
       <c r="B5">
-        <v>3.7810077999999998</v>
+        <v>9.7857140999999999</v>
       </c>
       <c r="C5">
-        <v>4.6763567999999998</v>
+        <v>1.9591837000000001</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A6">
-        <v>7.9707793999999996</v>
+        <v>11.643617000000001</v>
       </c>
       <c r="B6">
-        <v>8.4318179999999998</v>
+        <v>13.579787</v>
       </c>
       <c r="C6">
-        <v>7.5811687000000001</v>
+        <v>13.079787</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A7">
-        <v>12.201389000000001</v>
+        <v>2.0614754999999998</v>
       </c>
       <c r="B7">
-        <v>13.152778</v>
+        <v>3.1926228999999999</v>
       </c>
       <c r="C7">
-        <v>3.3611111999999999</v>
+        <v>3.8073771000000001</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A8">
-        <v>12.244872000000001</v>
+        <v>7.3235292000000003</v>
       </c>
       <c r="B8">
-        <v>8.8115386999999998</v>
+        <v>1.5</v>
       </c>
       <c r="C8">
-        <v>9.8961535000000005</v>
+        <v>11.595589</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A9">
-        <v>2.6636690999999999</v>
+        <v>13.22541</v>
       </c>
       <c r="B9">
-        <v>8.8507195000000003</v>
+        <v>10.70082</v>
       </c>
       <c r="C9">
-        <v>9.9478416000000003</v>
+        <v>12.151638999999999</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A10">
-        <v>4.7164178000000003</v>
+        <v>11.766949</v>
       </c>
       <c r="B10">
-        <v>2.5634329</v>
+        <v>1.1483051</v>
       </c>
       <c r="C10">
-        <v>13.208955</v>
+        <v>3.0805085000000001</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A11">
-        <v>3.4589553</v>
+        <v>13.385135</v>
       </c>
       <c r="B11">
-        <v>11.764925</v>
+        <v>7.2364864000000004</v>
       </c>
       <c r="C11">
-        <v>8.6604481</v>
+        <v>6.6554054999999996</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A12">
-        <v>9.8269234000000001</v>
+        <v>7.3666668</v>
       </c>
       <c r="B12">
-        <v>12.880769000000001</v>
+        <v>11.3</v>
       </c>
       <c r="C12">
-        <v>11.619230999999999</v>
+        <v>8.7666664000000001</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A13">
-        <v>9.3452377000000002</v>
+        <v>3.6083333</v>
       </c>
       <c r="B13">
-        <v>13.559524</v>
+        <v>12.083333</v>
       </c>
       <c r="C13">
-        <v>0.75</v>
+        <v>11.333333</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A14">
-        <v>10.583333</v>
+        <v>11.958955</v>
       </c>
       <c r="B14">
-        <v>11.638889000000001</v>
+        <v>12.160448000000001</v>
       </c>
       <c r="C14">
-        <v>12.379630000000001</v>
+        <v>0.94029850000000004</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A15">
-        <v>4.4642859000000001</v>
+        <v>2.0592104999999998</v>
       </c>
       <c r="B15">
-        <v>6.8785714999999996</v>
+        <v>10.118421</v>
       </c>
       <c r="C15">
-        <v>8.9214286999999999</v>
+        <v>3.7302632</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A16">
-        <v>1.1054217</v>
+        <v>13.356061</v>
       </c>
       <c r="B16">
-        <v>6.9728912999999997</v>
+        <v>5.6439395000000001</v>
       </c>
       <c r="C16">
-        <v>1.0331326000000001</v>
+        <v>8.8409089999999999</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A17">
-        <v>8.7313279999999995</v>
+        <v>0.97093021999999995</v>
       </c>
       <c r="B17">
-        <v>5.9118256999999996</v>
+        <v>7.6337209000000001</v>
       </c>
       <c r="C17">
-        <v>5.6545643999999999</v>
+        <v>3.5872092000000002</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A18">
-        <v>11.421429</v>
+        <v>2.9619564999999999</v>
       </c>
       <c r="B18">
-        <v>6.3214287999999996</v>
+        <v>5.9728260000000004</v>
       </c>
       <c r="C18">
-        <v>6.3428573999999998</v>
+        <v>0.97826086999999995</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A19">
-        <v>4.9543476000000002</v>
+        <v>13.460526</v>
       </c>
       <c r="B19">
-        <v>12.519565999999999</v>
+        <v>1.1184210999999999</v>
       </c>
       <c r="C19">
-        <v>13.028261000000001</v>
+        <v>11.881579</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A20">
-        <v>3.7976190999999999</v>
+        <v>8.3790320999999999</v>
       </c>
       <c r="B20">
-        <v>10.726191</v>
+        <v>3.7951611999999999</v>
       </c>
       <c r="C20">
-        <v>12.821427999999999</v>
+        <v>4.5016131000000001</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A21">
-        <v>4.2352942999999996</v>
+        <v>11.603659</v>
       </c>
       <c r="B21">
-        <v>5.2794118000000001</v>
+        <v>4.0060978</v>
       </c>
       <c r="C21">
-        <v>13.426470999999999</v>
+        <v>10.908537000000001</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A22">
-        <v>6.6689191000000001</v>
+        <v>9.0219296999999994</v>
       </c>
       <c r="B22">
-        <v>11.722973</v>
+        <v>1.0657894999999999</v>
       </c>
       <c r="C22">
-        <v>12.804054000000001</v>
+        <v>2.9868421999999999</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A23">
-        <v>8.9217175999999991</v>
+        <v>6.7688680000000003</v>
       </c>
       <c r="B23">
-        <v>4.1792932</v>
+        <v>12.75</v>
       </c>
       <c r="C23">
-        <v>1.0277778</v>
+        <v>12.627357999999999</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A24">
-        <v>4.3544774000000004</v>
+        <v>11.807693</v>
       </c>
       <c r="B24">
-        <v>13.451492</v>
+        <v>6.7692307999999999</v>
       </c>
       <c r="C24">
-        <v>10.660448000000001</v>
+        <v>1</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A25">
-        <v>12.773179000000001</v>
+        <v>3.7039472999999998</v>
       </c>
       <c r="B25">
-        <v>11.233442999999999</v>
+        <v>8.2105265000000003</v>
       </c>
       <c r="C25">
-        <v>1.2864237999999999</v>
+        <v>11.302631</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A26">
-        <v>12.797618999999999</v>
+        <v>0.87</v>
       </c>
       <c r="B26">
-        <v>10.535714</v>
+        <v>6.9299998</v>
       </c>
       <c r="C26">
-        <v>10.642858</v>
+        <v>2.0799998999999998</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A27">
-        <v>12.008620000000001</v>
+        <v>13.544117999999999</v>
       </c>
       <c r="B27">
-        <v>3.5172414999999999</v>
+        <v>13.632353</v>
       </c>
       <c r="C27">
-        <v>7.0344829999999998</v>
+        <v>10.044117999999999</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A28">
-        <v>9.5961542000000009</v>
+        <v>10.645833</v>
       </c>
       <c r="B28">
-        <v>5.7115383</v>
+        <v>7.7708335000000002</v>
       </c>
       <c r="C28">
-        <v>10.811539</v>
+        <v>8.7708329999999997</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A29">
-        <v>11.397057999999999</v>
+        <v>1.2470238</v>
       </c>
       <c r="B29">
-        <v>12.880252</v>
+        <v>8.0982140999999999</v>
       </c>
       <c r="C29">
-        <v>13.203780999999999</v>
+        <v>12.464286</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A30">
-        <v>5.8514495000000002</v>
+        <v>9.9866075999999993</v>
       </c>
       <c r="B30">
-        <v>4.9565215</v>
+        <v>6.7901787999999996</v>
       </c>
       <c r="C30">
-        <v>5.1702899999999996</v>
+        <v>2.9285714999999999</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A31">
-        <v>10.602739</v>
+        <v>4.6071429000000004</v>
       </c>
       <c r="B31">
-        <v>6.5821918999999998</v>
+        <v>9.3928575999999993</v>
       </c>
       <c r="C31">
-        <v>8.5650682000000007</v>
+        <v>2.8928571000000001</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A32">
-        <v>13.289773</v>
+        <v>11.626811999999999</v>
       </c>
       <c r="B32">
-        <v>4.3806820000000002</v>
+        <v>8.786232</v>
       </c>
       <c r="C32">
-        <v>6</v>
+        <v>1.134058</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A33">
-        <v>7.7094592999999998</v>
+        <v>10.771739</v>
       </c>
       <c r="B33">
-        <v>8.7860364999999998</v>
+        <v>9.3079710000000002</v>
       </c>
       <c r="C33">
-        <v>3.5472972</v>
+        <v>3.6775362</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A34">
-        <v>1.0925925999999999</v>
+        <v>6.4819589000000004</v>
       </c>
       <c r="B34">
-        <v>3.7638888000000001</v>
+        <v>11.507732000000001</v>
       </c>
       <c r="C34">
-        <v>8</v>
+        <v>3.9201031</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A35">
-        <v>10.211537999999999</v>
+        <v>0.91666669000000001</v>
       </c>
       <c r="B35">
-        <v>10.801282</v>
+        <v>5.3194447</v>
       </c>
       <c r="C35">
-        <v>10.096154</v>
+        <v>8.5694447</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A36">
-        <v>9.3385420000000003</v>
+        <v>8.9523811000000002</v>
       </c>
       <c r="B36">
-        <v>12.177083</v>
+        <v>0.75</v>
       </c>
       <c r="C36">
-        <v>6.28125</v>
+        <v>1.4761903999999999</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A37">
-        <v>7.4760871</v>
+        <v>1</v>
       </c>
       <c r="B37">
-        <v>8.8413047999999996</v>
+        <v>5.75</v>
       </c>
       <c r="C37">
-        <v>11.067391000000001</v>
+        <v>11.678572000000001</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A38">
-        <v>2.6973684000000002</v>
+        <v>3.5789472999999998</v>
       </c>
       <c r="B38">
-        <v>3.9122808</v>
+        <v>5.9835525000000001</v>
       </c>
       <c r="C38">
-        <v>9.9166670000000003</v>
+        <v>8.8256578000000001</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A39">
-        <v>2.9487950999999999</v>
+        <v>6.6808943999999997</v>
       </c>
       <c r="B39">
-        <v>0.73192769000000002</v>
+        <v>10.046747999999999</v>
       </c>
       <c r="C39">
-        <v>1.4487951999999999</v>
+        <v>6.1117887</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A40">
-        <v>3.7841879999999999</v>
+        <v>9.9642859000000001</v>
       </c>
       <c r="B40">
-        <v>6.3782053000000003</v>
+        <v>13.292857</v>
       </c>
       <c r="C40">
-        <v>11.967949000000001</v>
+        <v>0.59285712000000002</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A41">
-        <v>7.8427420000000003</v>
+        <v>5.7800001999999999</v>
       </c>
       <c r="B41">
-        <v>3.5564515999999999</v>
+        <v>5.4499997999999996</v>
       </c>
       <c r="C41">
-        <v>13.19758</v>
+        <v>7.02</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A42">
-        <v>10.033334</v>
+        <v>1.0714284999999999</v>
       </c>
       <c r="B42">
-        <v>8.1666670000000003</v>
+        <v>3.7559524</v>
       </c>
       <c r="C42">
-        <v>10.925000000000001</v>
+        <v>1.6547619</v>
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A43">
-        <v>6.5956788</v>
+        <v>11.675000000000001</v>
       </c>
       <c r="B43">
-        <v>9.0709876999999999</v>
+        <v>12.05</v>
       </c>
       <c r="C43">
-        <v>1.1265432</v>
+        <v>5.4499997999999996</v>
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A44">
-        <v>2.1041666999999999</v>
+        <v>6.0416664999999998</v>
       </c>
       <c r="B44">
-        <v>8.3020829999999997</v>
+        <v>4</v>
       </c>
       <c r="C44">
-        <v>7.9270835000000002</v>
+        <v>6.4583335000000002</v>
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A45">
-        <v>13.184343</v>
+        <v>3.6931818000000001</v>
       </c>
       <c r="B45">
-        <v>1.3661616000000001</v>
+        <v>4.8352275000000002</v>
       </c>
       <c r="C45">
-        <v>7.9469694999999998</v>
+        <v>2.8409089999999999</v>
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A46">
-        <v>10.659678</v>
+        <v>2.578125</v>
       </c>
       <c r="B46">
-        <v>8.8274193000000007</v>
+        <v>13.429688000000001</v>
       </c>
       <c r="C46">
-        <v>1.0532258000000001</v>
+        <v>7.0703125</v>
       </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A47">
-        <v>0.99193549000000003</v>
+        <v>7.7989511</v>
       </c>
       <c r="B47">
-        <v>9.4811831000000009</v>
+        <v>4.7604895000000003</v>
       </c>
       <c r="C47">
-        <v>7.2553763</v>
+        <v>1.2185315000000001</v>
       </c>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A48">
-        <v>5.6595744999999997</v>
+        <v>4.7094592999999998</v>
       </c>
       <c r="B48">
-        <v>0.95744680999999998</v>
+        <v>1.7837837999999999</v>
       </c>
       <c r="C48">
-        <v>0.89361703000000003</v>
+        <v>9.7297297</v>
       </c>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A49">
-        <v>2.8459596999999999</v>
+        <v>5.4625000999999997</v>
       </c>
       <c r="B49">
-        <v>9.9469700000000003</v>
+        <v>13.4</v>
       </c>
       <c r="C49">
-        <v>6.9166664999999998</v>
+        <v>7.4250002000000004</v>
       </c>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A50">
-        <v>0.859375</v>
+        <v>1.0107143000000001</v>
       </c>
       <c r="B50">
-        <v>13.53125</v>
+        <v>9.0428572000000003</v>
       </c>
       <c r="C50">
-        <v>12.890625</v>
+        <v>1.2071428</v>
       </c>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A51">
-        <v>9.6770829999999997</v>
+        <v>13.018966000000001</v>
       </c>
       <c r="B51">
-        <v>13.213542</v>
+        <v>1.587931</v>
       </c>
       <c r="C51">
-        <v>8.9010420000000003</v>
+        <v>5.8844829000000001</v>
       </c>
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A52">
-        <v>6.5166668999999997</v>
+        <v>0.89285713</v>
       </c>
       <c r="B52">
-        <v>7.1999997999999996</v>
+        <v>5.8928570999999996</v>
       </c>
       <c r="C52">
-        <v>1.6666666000000001</v>
+        <v>13.535714</v>
       </c>
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A53">
-        <v>7.9427709999999996</v>
+        <v>9.6163367999999991</v>
       </c>
       <c r="B53">
-        <v>0.70783132000000004</v>
+        <v>6.9628711000000001</v>
       </c>
       <c r="C53">
-        <v>8.0993977000000008</v>
+        <v>0.90841585000000002</v>
       </c>
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A54">
-        <v>13.523809</v>
+        <v>13.357142</v>
       </c>
       <c r="B54">
-        <v>1.9047619</v>
+        <v>13.160714</v>
       </c>
       <c r="C54">
-        <v>12.547618999999999</v>
+        <v>2.0625</v>
       </c>
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A55">
-        <v>13.119918999999999</v>
+        <v>0.93333334000000001</v>
       </c>
       <c r="B55">
-        <v>12.392277</v>
+        <v>5.8333335000000002</v>
       </c>
       <c r="C55">
-        <v>4.9044714000000003</v>
+        <v>12.616667</v>
       </c>
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A56">
-        <v>11.763514000000001</v>
+        <v>11.638158000000001</v>
       </c>
       <c r="B56">
-        <v>3.0472972</v>
+        <v>0.98026316999999996</v>
       </c>
       <c r="C56">
-        <v>0.64189189999999996</v>
+        <v>0.67105263000000004</v>
       </c>
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A57">
-        <v>3.9351851999999998</v>
+        <v>1.7971698</v>
       </c>
       <c r="B57">
-        <v>5.1388888000000001</v>
+        <v>12.858491000000001</v>
       </c>
       <c r="C57">
-        <v>4.8148150000000003</v>
+        <v>13.018867</v>
       </c>
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A58">
-        <v>9.6333331999999992</v>
+        <v>12.453882999999999</v>
       </c>
       <c r="B58">
-        <v>4.0777779000000001</v>
+        <v>13.415049</v>
       </c>
       <c r="C58">
-        <v>11.544444</v>
+        <v>6.6868930000000004</v>
       </c>
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A59">
-        <v>7.6373239000000002</v>
+        <v>9.4565219999999997</v>
       </c>
       <c r="B59">
-        <v>2.6936618999999999</v>
+        <v>2.0869564999999999</v>
       </c>
       <c r="C59">
-        <v>0.83450705000000003</v>
+        <v>12.260870000000001</v>
       </c>
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A60">
-        <v>13.513889000000001</v>
+        <v>10.416667</v>
       </c>
       <c r="B60">
-        <v>10.347222</v>
+        <v>5.8148150000000003</v>
       </c>
       <c r="C60">
-        <v>7.1527776999999997</v>
+        <v>11.342592</v>
       </c>
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A61">
-        <v>2.4469696999999999</v>
+        <v>5.6434913</v>
       </c>
       <c r="B61">
-        <v>5.8181820000000002</v>
+        <v>12.738166</v>
       </c>
       <c r="C61">
-        <v>12.5</v>
+        <v>5.5428996000000001</v>
       </c>
     </row>
     <row r="62" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A62">
-        <v>2.7045455</v>
+        <v>5.8543953999999996</v>
       </c>
       <c r="B62">
-        <v>4.9707793999999996</v>
+        <v>8.8269234000000001</v>
       </c>
       <c r="C62">
-        <v>0.87337661</v>
+        <v>12.486262999999999</v>
       </c>
     </row>
     <row r="63" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A63">
-        <v>0.80696201000000001</v>
+        <v>8.5654763999999997</v>
       </c>
       <c r="B63">
-        <v>0.83860760999999995</v>
+        <v>9.7857140999999999</v>
       </c>
       <c r="C63">
-        <v>2.4335444000000002</v>
+        <v>8.7261906000000007</v>
       </c>
     </row>
     <row r="64" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A64">
-        <v>7.0344829999999998</v>
+        <v>9.8697920000000003</v>
       </c>
       <c r="B64">
-        <v>2</v>
+        <v>3.8541666999999999</v>
       </c>
       <c r="C64">
-        <v>9.9224137999999993</v>
+        <v>11.770833</v>
       </c>
     </row>
     <row r="65" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A65">
-        <v>7.4000000999999997</v>
+        <v>1.0184211000000001</v>
       </c>
       <c r="B65">
-        <v>9.5500001999999995</v>
+        <v>8.8868417999999991</v>
       </c>
       <c r="C65">
-        <v>13.4</v>
+        <v>5.3184208999999996</v>
       </c>
     </row>
     <row r="66" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A66">
-        <v>9.6486482999999996</v>
+        <v>1.9237287999999999</v>
       </c>
       <c r="B66">
-        <v>1.8074323999999999</v>
+        <v>12.508474</v>
       </c>
       <c r="C66">
-        <v>10.716215999999999</v>
+        <v>2.0677967000000002</v>
       </c>
     </row>
     <row r="67" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A67">
-        <v>11.706522</v>
+        <v>12.552469</v>
       </c>
       <c r="B67">
-        <v>11.641304</v>
+        <v>1.0895060999999999</v>
       </c>
       <c r="C67">
-        <v>6.5326085000000003</v>
+        <v>9.7901229999999995</v>
       </c>
     </row>
     <row r="68" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A68">
-        <v>0.90909094000000001</v>
+        <v>6.9433961000000002</v>
       </c>
       <c r="B68">
-        <v>11.695455000000001</v>
+        <v>0.86320752000000001</v>
       </c>
       <c r="C68">
-        <v>6.1727271000000004</v>
+        <v>6.75</v>
       </c>
     </row>
     <row r="69" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A69">
-        <v>0.96428572999999995</v>
+        <v>7.9277778000000003</v>
       </c>
       <c r="B69">
-        <v>11.696427999999999</v>
+        <v>4.9277778000000003</v>
       </c>
       <c r="C69">
-        <v>2.9910714999999999</v>
+        <v>11.775926</v>
       </c>
     </row>
     <row r="70" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A70">
-        <v>5.7363014000000003</v>
+        <v>3.45</v>
       </c>
       <c r="B70">
-        <v>8.2157535999999993</v>
+        <v>12.676087000000001</v>
       </c>
       <c r="C70">
-        <v>13.277397000000001</v>
+        <v>4.8369565000000003</v>
       </c>
     </row>
     <row r="71" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A71">
-        <v>4.9258242000000001</v>
+        <v>6.6136365000000001</v>
       </c>
       <c r="B71">
-        <v>10.607142</v>
+        <v>4.8409089999999999</v>
       </c>
       <c r="C71">
-        <v>11.815934</v>
+        <v>2.8863637</v>
       </c>
     </row>
     <row r="72" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A72">
-        <v>9.7700005000000001</v>
+        <v>12.599463</v>
       </c>
       <c r="B72">
-        <v>8.8500004000000008</v>
+        <v>1.2123656</v>
       </c>
       <c r="C72">
-        <v>4.6799998</v>
+        <v>13.067204</v>
       </c>
     </row>
     <row r="73" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A73">
-        <v>7.6029410000000004</v>
+        <v>6.7785716000000003</v>
       </c>
       <c r="B73">
-        <v>11.441176</v>
+        <v>2.7714286000000001</v>
       </c>
       <c r="C73">
-        <v>1.3088236</v>
+        <v>6.7928572000000003</v>
       </c>
     </row>
     <row r="74" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A74">
-        <v>12.75</v>
+        <v>4.7790698999999996</v>
       </c>
       <c r="B74">
-        <v>6</v>
+        <v>7.8313950999999999</v>
       </c>
       <c r="C74">
-        <v>6.5</v>
+        <v>0.82558136999999998</v>
       </c>
     </row>
     <row r="75" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A75">
-        <v>10.59375</v>
+        <v>5.5914636</v>
       </c>
       <c r="B75">
-        <v>2.8348214999999999</v>
+        <v>11.737804000000001</v>
       </c>
       <c r="C75">
-        <v>1.9196428000000001</v>
+        <v>9.8963412999999996</v>
       </c>
     </row>
     <row r="76" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A76">
-        <v>11.093023000000001</v>
+        <v>11.818345000000001</v>
       </c>
       <c r="B76">
-        <v>5.2790698999999996</v>
+        <v>10.829136999999999</v>
       </c>
       <c r="C76">
-        <v>2.2616279000000001</v>
+        <v>3.2607913000000002</v>
       </c>
     </row>
     <row r="77" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A77">
-        <v>12.826389000000001</v>
+        <v>11.956250000000001</v>
       </c>
       <c r="B77">
-        <v>11.8125</v>
+        <v>4.03125</v>
       </c>
       <c r="C77">
-        <v>12.46875</v>
+        <v>8.7749995999999992</v>
       </c>
     </row>
     <row r="78" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A78">
-        <v>11.485294</v>
+        <v>5.4785713999999999</v>
       </c>
       <c r="B78">
-        <v>12.669117999999999</v>
+        <v>1.9738095</v>
       </c>
       <c r="C78">
-        <v>10.360294</v>
+        <v>7.9261904000000003</v>
       </c>
     </row>
     <row r="79" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A79">
-        <v>1.0669014000000001</v>
+        <v>8.9166670000000003</v>
       </c>
       <c r="B79">
-        <v>2.1021128</v>
+        <v>9.4166670000000003</v>
       </c>
       <c r="C79">
-        <v>9.8697186000000006</v>
+        <v>0.45833333999999998</v>
       </c>
     </row>
     <row r="80" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A80">
-        <v>5.7708335000000002</v>
+        <v>9.5456991000000002</v>
       </c>
       <c r="B80">
-        <v>4.0972223000000003</v>
+        <v>3.6559140999999999</v>
       </c>
       <c r="C80">
-        <v>0.8125</v>
+        <v>8.9758061999999992</v>
       </c>
     </row>
     <row r="81" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A81">
-        <v>11.322464</v>
+        <v>0.85185188000000001</v>
       </c>
       <c r="B81">
-        <v>6.4456519999999999</v>
+        <v>9.4629630999999996</v>
       </c>
       <c r="C81">
-        <v>10.844203</v>
+        <v>9.8148146000000001</v>
       </c>
     </row>
     <row r="82" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A82">
-        <v>9.5512818999999993</v>
+        <v>11.905340000000001</v>
       </c>
       <c r="B82">
-        <v>8.7307691999999992</v>
+        <v>1.8325243</v>
       </c>
       <c r="C82">
-        <v>8.6730765999999999</v>
+        <v>8.3033981000000008</v>
       </c>
     </row>
     <row r="83" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A83">
-        <v>6.8400002000000004</v>
+        <v>12.026596</v>
       </c>
       <c r="B83">
-        <v>8.5649996000000002</v>
+        <v>12.063829</v>
       </c>
       <c r="C83">
-        <v>4.9650002000000004</v>
+        <v>13.244680000000001</v>
       </c>
     </row>
     <row r="84" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A84">
-        <v>13.520833</v>
+        <v>12.757936000000001</v>
       </c>
       <c r="B84">
-        <v>2.5416666999999999</v>
+        <v>12.988095</v>
       </c>
       <c r="C84">
-        <v>4</v>
+        <v>3.8293650000000001</v>
       </c>
     </row>
     <row r="85" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A85">
-        <v>0.83771932000000005</v>
+        <v>13.576923000000001</v>
       </c>
       <c r="B85">
-        <v>11.328946999999999</v>
+        <v>3.2115385999999999</v>
       </c>
       <c r="C85">
-        <v>9.7982454000000008</v>
+        <v>3.7884614000000001</v>
       </c>
     </row>
     <row r="86" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A86">
-        <v>13.022727</v>
+        <v>0.65972220999999998</v>
       </c>
       <c r="B86">
-        <v>13.397727</v>
+        <v>3.7430555999999999</v>
       </c>
       <c r="C86">
-        <v>10.034091</v>
+        <v>6.7847223000000003</v>
       </c>
     </row>
     <row r="87" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A87">
-        <v>0.82446808000000005</v>
+        <v>6.7094592999999998</v>
       </c>
       <c r="B87">
-        <v>5.4521274999999996</v>
+        <v>6.6486486999999999</v>
       </c>
       <c r="C87">
-        <v>13.218085</v>
+        <v>9.8378382000000002</v>
       </c>
     </row>
     <row r="88" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A88">
-        <v>12.880682</v>
+        <v>9.046875</v>
       </c>
       <c r="B88">
-        <v>8.6818179999999998</v>
+        <v>13.058593999999999</v>
       </c>
       <c r="C88">
-        <v>12.954545</v>
+        <v>2.1289063000000001</v>
       </c>
     </row>
     <row r="89" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A89">
-        <v>5.5783582000000003</v>
+        <v>6.4814816000000004</v>
       </c>
       <c r="B89">
-        <v>8.7873134999999998</v>
+        <v>7.6296296000000003</v>
       </c>
       <c r="C89">
-        <v>6.8022388999999999</v>
+        <v>13.361110999999999</v>
       </c>
     </row>
     <row r="90" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A90">
-        <v>1.1796297</v>
+        <v>3.6822032999999998</v>
       </c>
       <c r="B90">
-        <v>3.7314816</v>
+        <v>8.6483048999999994</v>
       </c>
       <c r="C90">
-        <v>5.6907405999999998</v>
+        <v>6.9872880000000004</v>
       </c>
     </row>
     <row r="91" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A91">
-        <v>10.29</v>
+        <v>3.8736557999999999</v>
       </c>
       <c r="B91">
-        <v>4.5100002000000003</v>
+        <v>3.9381721000000001</v>
       </c>
       <c r="C91">
-        <v>2.8299998999999998</v>
+        <v>5.7553763</v>
       </c>
     </row>
     <row r="92" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A92">
-        <v>13.434210999999999</v>
+        <v>9.7672415000000008</v>
       </c>
       <c r="B92">
-        <v>7.8289474999999999</v>
+        <v>12.818966</v>
       </c>
       <c r="C92">
-        <v>8.0657891999999993</v>
+        <v>3.2844826999999999</v>
       </c>
     </row>
     <row r="93" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A93">
-        <v>6.3189653999999997</v>
+        <v>10.75</v>
       </c>
       <c r="B93">
-        <v>1.0431035</v>
+        <v>2.425926</v>
       </c>
       <c r="C93">
-        <v>13.560345</v>
+        <v>1.0185185999999999</v>
       </c>
     </row>
     <row r="94" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A94">
-        <v>10.960526</v>
+        <v>1.7826797999999999</v>
       </c>
       <c r="B94">
-        <v>9.9254388999999996</v>
+        <v>1.2892157</v>
       </c>
       <c r="C94">
-        <v>12.065789000000001</v>
+        <v>1.0310458</v>
       </c>
     </row>
     <row r="95" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A95">
-        <v>13.345238</v>
+        <v>6.7907409999999997</v>
       </c>
       <c r="B95">
-        <v>10.107142</v>
+        <v>3.6537036999999999</v>
       </c>
       <c r="C95">
-        <v>13.273809</v>
+        <v>10.546296</v>
       </c>
     </row>
     <row r="96" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A96">
-        <v>5.6041664999999998</v>
+        <v>2.4027777000000001</v>
       </c>
       <c r="B96">
-        <v>6.3125</v>
+        <v>9.7361106999999993</v>
       </c>
       <c r="C96">
-        <v>9.2291670000000003</v>
+        <v>1.8055555999999999</v>
       </c>
     </row>
     <row r="97" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A97">
-        <v>10.596939000000001</v>
+        <v>10.633333</v>
       </c>
       <c r="B97">
-        <v>2.3928571000000001</v>
+        <v>10.75</v>
       </c>
       <c r="C97">
-        <v>4.6377549</v>
+        <v>5.6833334000000004</v>
       </c>
     </row>
     <row r="98" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A98">
-        <v>3.1866197999999999</v>
+        <v>7.9110575000000001</v>
       </c>
       <c r="B98">
-        <v>6.1443662999999997</v>
+        <v>4.8485575000000001</v>
       </c>
       <c r="C98">
-        <v>7.8556337000000003</v>
+        <v>6.9543271000000004</v>
       </c>
     </row>
     <row r="99" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A99">
-        <v>11.710526</v>
+        <v>3.8986486999999999</v>
       </c>
       <c r="B99">
-        <v>5.6184210999999999</v>
+        <v>4.3716216000000001</v>
       </c>
       <c r="C99">
-        <v>0.61842107999999996</v>
+        <v>7.6891889999999998</v>
       </c>
     </row>
     <row r="100" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A100">
-        <v>8.6451615999999998</v>
+        <v>2.7205881999999999</v>
       </c>
       <c r="B100">
-        <v>5.3548387999999996</v>
+        <v>8.5588236000000002</v>
       </c>
       <c r="C100">
-        <v>12.362904</v>
+        <v>0.76470590000000005</v>
       </c>
     </row>
     <row r="101" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A101">
-        <v>10.5</v>
+        <v>6.25</v>
       </c>
       <c r="B101">
-        <v>5.6477275000000002</v>
+        <v>9.1666670000000003</v>
       </c>
       <c r="C101">
-        <v>13.340909</v>
+        <v>2.8134920999999999</v>
       </c>
     </row>
     <row r="102" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A102">
-        <v>8.8701553000000004</v>
+        <v>1.0718391</v>
       </c>
       <c r="B102">
-        <v>11.052325</v>
+        <v>5.1120691000000003</v>
       </c>
       <c r="C102">
-        <v>9.2771319999999999</v>
+        <v>10.227012</v>
       </c>
     </row>
     <row r="103" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A103">
-        <v>0.93292682999999998</v>
+        <v>11.117925</v>
       </c>
       <c r="B103">
-        <v>3.054878</v>
+        <v>5.8066038999999998</v>
       </c>
       <c r="C103">
-        <v>11.408537000000001</v>
+        <v>1.2877358000000001</v>
       </c>
     </row>
     <row r="104" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A104">
-        <v>6.9463471999999999</v>
+        <v>5.9383115999999996</v>
       </c>
       <c r="B104">
-        <v>2.9006848000000001</v>
+        <v>0.92532468000000001</v>
       </c>
       <c r="C104">
-        <v>2.9394977</v>
+        <v>12.730518999999999</v>
       </c>
     </row>
     <row r="105" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A105">
-        <v>13.345238</v>
+        <v>2.8344157000000001</v>
       </c>
       <c r="B105">
-        <v>1.3849206000000001</v>
+        <v>2.9058442000000002</v>
       </c>
       <c r="C105">
-        <v>5.2976188999999998</v>
+        <v>12.009740000000001</v>
       </c>
     </row>
     <row r="106" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A106">
-        <v>4.1944447</v>
+        <v>0.67372882000000001</v>
       </c>
       <c r="B106">
-        <v>0.75</v>
+        <v>10.377119</v>
       </c>
       <c r="C106">
-        <v>3.9166666999999999</v>
+        <v>3.5720339000000001</v>
       </c>
     </row>
     <row r="107" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A107">
-        <v>8.9578647999999994</v>
+        <v>3.8892045</v>
       </c>
       <c r="B107">
-        <v>6.8426967000000003</v>
+        <v>11.883523</v>
       </c>
       <c r="C107">
-        <v>1.8792135000000001</v>
+        <v>8.0397730000000003</v>
       </c>
     </row>
     <row r="108" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A108">
-        <v>9.0826615999999998</v>
+        <v>11.632353</v>
       </c>
       <c r="B108">
-        <v>11.356854</v>
+        <v>0.65196078999999996</v>
       </c>
       <c r="C108">
-        <v>3.1028224999999998</v>
+        <v>6.0931373000000004</v>
       </c>
     </row>
     <row r="109" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A109">
-        <v>0.81756759000000001</v>
+        <v>11.850529</v>
       </c>
       <c r="B109">
-        <v>10.412162</v>
+        <v>3.7949736000000001</v>
       </c>
       <c r="C109">
-        <v>0.85810810000000004</v>
+        <v>5.8505292000000004</v>
       </c>
     </row>
     <row r="110" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A110">
-        <v>2.8911764999999998</v>
+        <v>1.2153678999999999</v>
       </c>
       <c r="B110">
-        <v>10.244118</v>
+        <v>1.6937230000000001</v>
       </c>
       <c r="C110">
-        <v>4.1558824000000003</v>
+        <v>3.7456710000000002</v>
       </c>
     </row>
     <row r="111" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A111">
-        <v>1.8686868999999999</v>
+        <v>9.0335053999999992</v>
       </c>
       <c r="B111">
-        <v>6.2095962</v>
+        <v>12.46134</v>
       </c>
       <c r="C111">
-        <v>5.1464648000000004</v>
+        <v>12.489691000000001</v>
       </c>
     </row>
     <row r="112" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A112">
-        <v>1.3976189999999999</v>
+        <v>4.0755815999999996</v>
       </c>
       <c r="B112">
-        <v>13.045237999999999</v>
+        <v>0.76162790999999996</v>
       </c>
       <c r="C112">
-        <v>1.2452380999999999</v>
+        <v>10.843023000000001</v>
       </c>
     </row>
     <row r="113" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A113">
-        <v>1.96875</v>
+        <v>3.6753730999999998</v>
       </c>
       <c r="B113">
-        <v>6.8125</v>
+        <v>1.9962686000000001</v>
       </c>
       <c r="C113">
-        <v>13.5</v>
+        <v>3.4813432999999998</v>
       </c>
     </row>
     <row r="114" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A114">
-        <v>1.2023809000000001</v>
+        <v>0.77205884000000002</v>
       </c>
       <c r="B114">
-        <v>5.7785716000000003</v>
+        <v>2.3602941</v>
       </c>
       <c r="C114">
-        <v>2.0119047000000001</v>
+        <v>10.713234999999999</v>
       </c>
     </row>
     <row r="115" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A115">
-        <v>6.7137098000000002</v>
+        <v>12.943548</v>
       </c>
       <c r="B115">
-        <v>1.0282258</v>
+        <v>10.787635</v>
       </c>
       <c r="C115">
-        <v>11.842741999999999</v>
+        <v>7.0887098000000002</v>
       </c>
     </row>
     <row r="116" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A116">
-        <v>6.5182928999999996</v>
+        <v>11.273255000000001</v>
       </c>
       <c r="B116">
-        <v>3.7560975999999999</v>
+        <v>2.0988370999999999</v>
       </c>
       <c r="C116">
-        <v>8.5914631000000004</v>
+        <v>12.273255000000001</v>
       </c>
     </row>
     <row r="117" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A117">
-        <v>2.6940298</v>
+        <v>1.6650944000000001</v>
       </c>
       <c r="B117">
-        <v>11.488806</v>
+        <v>2.8915095000000002</v>
       </c>
       <c r="C117">
-        <v>1.2089551999999999</v>
+        <v>8.7264146999999994</v>
       </c>
     </row>
     <row r="118" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A118">
-        <v>4.9772724999999998</v>
+        <v>1.8846153999999999</v>
       </c>
       <c r="B118">
-        <v>8.3787880000000001</v>
+        <v>8.6730765999999999</v>
       </c>
       <c r="C118">
-        <v>2.3333333000000001</v>
+        <v>10.673076999999999</v>
       </c>
     </row>
     <row r="119" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A119">
-        <v>11.25</v>
+        <v>3.6681819</v>
       </c>
       <c r="B119">
-        <v>6.5357140999999999</v>
+        <v>6.0954547000000003</v>
       </c>
       <c r="C119">
-        <v>4.6071429000000004</v>
+        <v>13.340909</v>
       </c>
     </row>
     <row r="120" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A120">
-        <v>4.5379747999999998</v>
+        <v>1.3401639000000001</v>
       </c>
       <c r="B120">
-        <v>7.0854429999999997</v>
+        <v>0.84836065999999999</v>
       </c>
       <c r="C120">
-        <v>0.94936710999999996</v>
+        <v>11.610656000000001</v>
       </c>
     </row>
     <row r="121" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A121">
-        <v>4.0967741000000002</v>
+        <v>13.607142</v>
       </c>
       <c r="B121">
-        <v>12.959678</v>
+        <v>8.8214283000000009</v>
       </c>
       <c r="C121">
-        <v>1.0564515999999999</v>
+        <v>3.5357143999999998</v>
       </c>
     </row>
     <row r="122" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A122">
-        <v>11.714028000000001</v>
+        <v>6.6458335000000002</v>
       </c>
       <c r="B122">
-        <v>1.0017985</v>
+        <v>5.9375</v>
       </c>
       <c r="C122">
-        <v>3.7464029999999999</v>
+        <v>12.840278</v>
       </c>
     </row>
     <row r="123" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A123">
-        <v>6.5394734999999997</v>
+        <v>6.1206899000000003</v>
       </c>
       <c r="B123">
-        <v>8.0921049000000007</v>
+        <v>1.612069</v>
       </c>
       <c r="C123">
-        <v>6.1184210999999999</v>
+        <v>9.9741382999999999</v>
       </c>
     </row>
     <row r="124" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A124">
-        <v>13.525862</v>
+        <v>3.7981482</v>
       </c>
       <c r="B124">
-        <v>11.715517</v>
+        <v>5.8574076000000002</v>
       </c>
       <c r="C124">
-        <v>7.9568968</v>
+        <v>11.603702999999999</v>
       </c>
     </row>
     <row r="125" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A125">
-        <v>2.7923729000000002</v>
+        <v>11.106</v>
       </c>
       <c r="B125">
-        <v>8.8177967000000006</v>
+        <v>6.4660000999999996</v>
       </c>
       <c r="C125">
-        <v>0.74152541000000005</v>
+        <v>4.8019999999999996</v>
       </c>
     </row>
     <row r="126" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A126">
-        <v>5.5935116000000003</v>
+        <v>10.941011</v>
       </c>
       <c r="B126">
-        <v>9.9370232000000005</v>
+        <v>3.9634830999999999</v>
       </c>
       <c r="C126">
-        <v>8.9408397999999991</v>
+        <v>1.1095505999999999</v>
       </c>
     </row>
     <row r="127" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A127">
-        <v>10.897826</v>
+        <v>13.098485</v>
       </c>
       <c r="B127">
-        <v>11.089130000000001</v>
+        <v>8.8762626999999998</v>
       </c>
       <c r="C127">
-        <v>8.0934781999999998</v>
+        <v>4.4772724999999998</v>
       </c>
     </row>
     <row r="128" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A128">
-        <v>2.6722220999999999</v>
+        <v>4.0725807999999999</v>
       </c>
       <c r="B128">
-        <v>3.7722223000000001</v>
+        <v>3.7419354999999999</v>
       </c>
       <c r="C128">
-        <v>12.744445000000001</v>
+        <v>3.9274193999999998</v>
       </c>
     </row>
     <row r="129" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A129">
-        <v>0.84803921000000004</v>
+        <v>8.4598216999999991</v>
       </c>
       <c r="B129">
-        <v>8.9362744999999997</v>
+        <v>9.6741075999999993</v>
       </c>
       <c r="C129">
-        <v>1.0931373</v>
+        <v>11.4375</v>
       </c>
     </row>
     <row r="130" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A130">
-        <v>11.057017</v>
+        <v>10.311225</v>
       </c>
       <c r="B130">
-        <v>13.153509</v>
+        <v>0.99489795999999997</v>
       </c>
       <c r="C130">
-        <v>5.4692983999999996</v>
+        <v>13.392858</v>
       </c>
     </row>
     <row r="131" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A131">
-        <v>2.2000000000000002</v>
+        <v>1.0373564</v>
       </c>
       <c r="B131">
-        <v>1.0700000999999999</v>
+        <v>5.0890803</v>
       </c>
       <c r="C131">
-        <v>8.5</v>
+        <v>4.1293100999999997</v>
       </c>
     </row>
     <row r="132" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A132">
-        <v>0.90517241000000004</v>
+        <v>5.9078945999999997</v>
       </c>
       <c r="B132">
-        <v>3.2327585000000001</v>
+        <v>7.2236843000000004</v>
       </c>
       <c r="C132">
-        <v>13.025862</v>
+        <v>6.8728069999999999</v>
       </c>
     </row>
     <row r="133" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A133">
-        <v>3.7236842999999999</v>
+        <v>3.0247251999999998</v>
       </c>
       <c r="B133">
-        <v>3</v>
+        <v>10.326923000000001</v>
       </c>
       <c r="C133">
-        <v>5.0570173</v>
+        <v>13.14011</v>
       </c>
     </row>
     <row r="134" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A134">
-        <v>1.0537974999999999</v>
+        <v>8</v>
       </c>
       <c r="B134">
-        <v>3.8702530999999998</v>
+        <v>0.78571427000000005</v>
       </c>
       <c r="C134">
-        <v>2.9272151000000002</v>
+        <v>12.946427999999999</v>
       </c>
     </row>
     <row r="135" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A135">
-        <v>7.7990197999999999</v>
+        <v>0.95270270000000001</v>
       </c>
       <c r="B135">
-        <v>12.887255</v>
+        <v>13.128378</v>
       </c>
       <c r="C135">
-        <v>10.436275</v>
+        <v>8.1621617999999998</v>
       </c>
     </row>
     <row r="136" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A136">
-        <v>9.7079830000000005</v>
+        <v>4.7628206999999998</v>
       </c>
       <c r="B136">
-        <v>1.0021008</v>
+        <v>1.0961539</v>
       </c>
       <c r="C136">
-        <v>0.95588236999999998</v>
+        <v>2.4551281999999999</v>
       </c>
     </row>
     <row r="137" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A137">
-        <v>10.69</v>
+        <v>13.278302</v>
       </c>
       <c r="B137">
-        <v>4.8699998999999998</v>
+        <v>6.6556601999999998</v>
       </c>
       <c r="C137">
-        <v>4.5900002000000004</v>
+        <v>5.0801888000000002</v>
       </c>
     </row>
     <row r="138" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A138">
-        <v>13.318966</v>
+        <v>0.91470587000000003</v>
       </c>
       <c r="B138">
-        <v>8.3965520999999992</v>
+        <v>10.767647</v>
       </c>
       <c r="C138">
-        <v>3.2413793000000002</v>
+        <v>8.7147055000000009</v>
       </c>
     </row>
     <row r="139" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A139">
-        <v>0.93000000999999999</v>
+        <v>7.03125</v>
       </c>
       <c r="B139">
-        <v>9.8140000999999994</v>
+        <v>6.0625</v>
       </c>
       <c r="C139">
-        <v>3.6140001000000002</v>
+        <v>6.65625</v>
       </c>
     </row>
     <row r="140" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A140">
-        <v>1.2604895</v>
+        <v>3.7111649999999998</v>
       </c>
       <c r="B140">
-        <v>11.882866999999999</v>
+        <v>10.036407000000001</v>
       </c>
       <c r="C140">
-        <v>12.529719999999999</v>
+        <v>10.929611</v>
       </c>
     </row>
     <row r="141" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A141">
-        <v>6.4250002000000004</v>
+        <v>9.0153847000000003</v>
       </c>
       <c r="B141">
-        <v>6.2249999000000003</v>
+        <v>13.373077</v>
       </c>
       <c r="C141">
-        <v>7.75</v>
+        <v>8.9576920999999992</v>
       </c>
     </row>
     <row r="142" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A142">
-        <v>0.98584908000000004</v>
+        <v>5.8939395000000001</v>
       </c>
       <c r="B142">
-        <v>13.278302</v>
+        <v>5.5530305000000002</v>
       </c>
       <c r="C142">
-        <v>5.0613207999999998</v>
+        <v>8.8257580000000004</v>
       </c>
     </row>
     <row r="143" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A143">
-        <v>5.9782609999999998</v>
+        <v>1.8686441</v>
       </c>
       <c r="B143">
-        <v>1.5942029</v>
+        <v>6.0127119999999996</v>
       </c>
       <c r="C143">
-        <v>7.1920289999999998</v>
+        <v>2.4110168999999999</v>
       </c>
     </row>
     <row r="144" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A144">
-        <v>11.729638</v>
+        <v>12.162463000000001</v>
       </c>
       <c r="B144">
-        <v>9.8563346999999997</v>
+        <v>12.198071000000001</v>
       </c>
       <c r="C144">
-        <v>3.8880091000000001</v>
+        <v>10.031898999999999</v>
       </c>
     </row>
     <row r="145" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A145">
-        <v>8.3529415</v>
+        <v>6.4739585000000002</v>
       </c>
       <c r="B145">
-        <v>13.397057999999999</v>
+        <v>3.5729166999999999</v>
       </c>
       <c r="C145">
-        <v>3.3970587000000001</v>
+        <v>3.7708333000000001</v>
       </c>
     </row>
     <row r="146" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A146">
-        <v>10.889343999999999</v>
+        <v>5.9817071000000004</v>
       </c>
       <c r="B146">
-        <v>0.93032789000000005</v>
+        <v>10.554878</v>
       </c>
       <c r="C146">
-        <v>12.889343999999999</v>
+        <v>1.054878</v>
       </c>
     </row>
     <row r="147" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A147">
-        <v>7.8430232999999996</v>
+        <v>1.7258065</v>
       </c>
       <c r="B147">
-        <v>13.401163</v>
+        <v>4.3306450999999999</v>
       </c>
       <c r="C147">
-        <v>12.459301999999999</v>
+        <v>13.419354</v>
       </c>
     </row>
     <row r="148" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A148">
-        <v>12.962121</v>
+        <v>0.47499998999999998</v>
       </c>
       <c r="B148">
-        <v>10.840909</v>
+        <v>10.425000000000001</v>
       </c>
       <c r="C148">
-        <v>2.9469696999999999</v>
+        <v>7.1999997999999996</v>
       </c>
     </row>
     <row r="149" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A149">
-        <v>13.464286</v>
+        <v>7.7134147000000004</v>
       </c>
       <c r="B149">
-        <v>5.8035712000000004</v>
+        <v>9.9817076</v>
       </c>
       <c r="C149">
-        <v>4.2142859000000001</v>
+        <v>13.408537000000001</v>
       </c>
     </row>
     <row r="150" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A150">
-        <v>4.4078945999999997</v>
+        <v>13.003333</v>
       </c>
       <c r="B150">
-        <v>6.8903508000000002</v>
+        <v>6.8366666</v>
       </c>
       <c r="C150">
-        <v>3.4166666999999999</v>
+        <v>12.683332999999999</v>
       </c>
     </row>
     <row r="151" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A151">
-        <v>12.701389000000001</v>
+        <v>9.836957</v>
       </c>
       <c r="B151">
-        <v>12.756945</v>
+        <v>4.9782609999999998</v>
       </c>
       <c r="C151">
-        <v>6.9236111999999999</v>
+        <v>3.8369564999999999</v>
       </c>
     </row>
     <row r="152" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A152">
-        <v>8.7979450000000003</v>
+        <v>1.0036764</v>
       </c>
       <c r="B152">
-        <v>9.0513697000000004</v>
+        <v>6.7352942999999996</v>
       </c>
       <c r="C152">
-        <v>5.9212327</v>
+        <v>6.0551472000000004</v>
       </c>
     </row>
     <row r="153" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A153">
-        <v>4.8353657999999999</v>
+        <v>5.9115386000000001</v>
       </c>
       <c r="B153">
-        <v>6.7804880000000001</v>
+        <v>2.8269231000000001</v>
       </c>
       <c r="C153">
-        <v>6.5243902</v>
+        <v>12.657692000000001</v>
       </c>
     </row>
     <row r="154" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A154">
-        <v>2.0192307999999999</v>
+        <v>10.511628</v>
       </c>
       <c r="B154">
-        <v>13.416667</v>
+        <v>12.040698000000001</v>
       </c>
       <c r="C154">
-        <v>11.532050999999999</v>
+        <v>6.9069767000000004</v>
       </c>
     </row>
     <row r="155" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A155">
-        <v>13.266394</v>
+        <v>12.764851999999999</v>
       </c>
       <c r="B155">
-        <v>4.3237705000000002</v>
+        <v>3.0420791999999999</v>
       </c>
       <c r="C155">
-        <v>0.71721309</v>
+        <v>11.155941</v>
       </c>
     </row>
     <row r="156" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A156">
-        <v>6.8611111999999999</v>
+        <v>1.2424242000000001</v>
       </c>
       <c r="B156">
-        <v>0.8125</v>
+        <v>11.511364</v>
       </c>
       <c r="C156">
-        <v>3.9444444000000001</v>
+        <v>6.3409089999999999</v>
       </c>
     </row>
     <row r="157" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A157">
-        <v>13.392858</v>
+        <v>12.835227</v>
       </c>
       <c r="B157">
-        <v>13.321427999999999</v>
+        <v>10.454545</v>
       </c>
       <c r="C157">
-        <v>0.25</v>
+        <v>5.2272724999999998</v>
       </c>
     </row>
     <row r="158" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A158">
-        <v>4.2708335000000002</v>
+        <v>8.6997490000000006</v>
       </c>
       <c r="B158">
-        <v>8.2847223000000003</v>
+        <v>6.8655777000000002</v>
       </c>
       <c r="C158">
-        <v>8.1111106999999993</v>
+        <v>10.089195999999999</v>
       </c>
     </row>
     <row r="159" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A159">
-        <v>12.657692000000001</v>
+        <v>6.5878376999999997</v>
       </c>
       <c r="B159">
-        <v>5.4423075000000001</v>
+        <v>12.763514000000001</v>
       </c>
       <c r="C159">
-        <v>7.4038462999999997</v>
+        <v>8.8175678000000008</v>
       </c>
     </row>
     <row r="160" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A160">
-        <v>13.347939</v>
+        <v>8.9026718000000002</v>
       </c>
       <c r="B160">
-        <v>5.3479381000000004</v>
+        <v>12.875954999999999</v>
       </c>
       <c r="C160">
-        <v>9.6984539000000005</v>
+        <v>5.5667939000000004</v>
       </c>
     </row>
     <row r="161" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A161">
-        <v>12.425879</v>
+        <v>5.8881763999999999</v>
       </c>
       <c r="B161">
-        <v>1.0716081</v>
+        <v>8.9408835999999994</v>
       </c>
       <c r="C161">
-        <v>11.199749000000001</v>
+        <v>9.5548429000000006</v>
       </c>
     </row>
     <row r="162" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A162">
-        <v>13.447369</v>
+        <v>5.3703703999999997</v>
       </c>
       <c r="B162">
-        <v>11.842105</v>
+        <v>13.361110999999999</v>
       </c>
       <c r="C162">
-        <v>10.552631</v>
+        <v>9.6296301</v>
       </c>
     </row>
     <row r="163" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A163">
-        <v>9.5147057000000004</v>
+        <v>6.0192307999999999</v>
       </c>
       <c r="B163">
-        <v>8.4068632000000001</v>
+        <v>13.538462000000001</v>
       </c>
       <c r="C163">
-        <v>12.696078</v>
+        <v>13.403846</v>
       </c>
     </row>
     <row r="164" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A164">
-        <v>4.0247935999999997</v>
+        <v>3.8289472999999998</v>
       </c>
       <c r="B164">
-        <v>4.3202480999999997</v>
+        <v>3.5438597000000001</v>
       </c>
       <c r="C164">
-        <v>8.0557852000000008</v>
+        <v>1.0175438999999999</v>
       </c>
     </row>
     <row r="165" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A165">
-        <v>0.97222220999999998</v>
+        <v>3.5094935999999999</v>
       </c>
       <c r="B165">
-        <v>8.1540403000000001</v>
+        <v>6.6803799000000001</v>
       </c>
       <c r="C165">
-        <v>13.022727</v>
+        <v>5.8322782999999996</v>
       </c>
     </row>
     <row r="166" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A166">
-        <v>10.555555</v>
+        <v>0.75724638</v>
       </c>
       <c r="B166">
-        <v>6.8888888000000001</v>
+        <v>12.438406000000001</v>
       </c>
       <c r="C166">
-        <v>3.7407408000000002</v>
+        <v>0.89492755999999996</v>
       </c>
     </row>
     <row r="167" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A167">
-        <v>4.125</v>
+        <v>4.6458335000000002</v>
       </c>
       <c r="B167">
-        <v>8.4305553</v>
+        <v>7.6666664999999998</v>
       </c>
       <c r="C167">
-        <v>4.6296296000000003</v>
+        <v>2.6666666999999999</v>
       </c>
     </row>
     <row r="168" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A168">
-        <v>7.7701149000000003</v>
+        <v>11.75</v>
       </c>
       <c r="B168">
-        <v>6.5373564000000002</v>
+        <v>5.7916664999999998</v>
       </c>
       <c r="C168">
-        <v>9.8275862000000007</v>
+        <v>11.638889000000001</v>
       </c>
     </row>
     <row r="169" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A169">
-        <v>0.95129870999999999</v>
+        <v>9.8788661999999992</v>
       </c>
       <c r="B169">
-        <v>4.7824673999999998</v>
+        <v>9.9149484999999995</v>
       </c>
       <c r="C169">
-        <v>10.931818</v>
+        <v>1.1520618</v>
       </c>
     </row>
     <row r="170" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A170">
-        <v>7.3396224999999999</v>
+        <v>1.0247253000000001</v>
       </c>
       <c r="B170">
-        <v>5.4528302999999996</v>
+        <v>12.898351999999999</v>
       </c>
       <c r="C170">
-        <v>7.7594336999999998</v>
+        <v>4.5302195999999997</v>
       </c>
     </row>
     <row r="171" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A171">
-        <v>7.1812500999999997</v>
+        <v>2.3474026000000001</v>
       </c>
       <c r="B171">
-        <v>10.36875</v>
+        <v>12.925324</v>
       </c>
       <c r="C171">
-        <v>9.5249995999999992</v>
+        <v>10.555194999999999</v>
       </c>
     </row>
     <row r="172" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A172">
-        <v>3.6318182999999999</v>
+        <v>3.7246377000000002</v>
       </c>
       <c r="B172">
-        <v>0.98333334999999999</v>
+        <v>10.115942</v>
       </c>
       <c r="C172">
-        <v>10.916667</v>
+        <v>5.6739129999999998</v>
       </c>
     </row>
     <row r="173" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A173">
-        <v>5.7249999000000003</v>
+        <v>4.9435482000000004</v>
       </c>
       <c r="B173">
-        <v>10.25</v>
+        <v>9.0564517999999996</v>
       </c>
       <c r="C173">
-        <v>5.8000002000000004</v>
+        <v>13.620968</v>
       </c>
     </row>
     <row r="174" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A174">
-        <v>6.3306450999999999</v>
+        <v>11.735075</v>
       </c>
       <c r="B174">
-        <v>0.62096775000000004</v>
+        <v>9.8843279000000006</v>
       </c>
       <c r="C174">
-        <v>5.7177420000000003</v>
+        <v>13.108209</v>
       </c>
     </row>
     <row r="175" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A175">
-        <v>12.838785</v>
+        <v>11.044737</v>
       </c>
       <c r="B175">
-        <v>1.021028</v>
+        <v>6.9499997999999996</v>
       </c>
       <c r="C175">
-        <v>1.2920560999999999</v>
+        <v>10.086843</v>
       </c>
     </row>
     <row r="176" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A176">
-        <v>0.40789472999999998</v>
+        <v>12.809524</v>
       </c>
       <c r="B176">
-        <v>7.5394734999999997</v>
+        <v>12.452381000000001</v>
       </c>
       <c r="C176">
-        <v>11.539474</v>
+        <v>6.6904763999999997</v>
       </c>
     </row>
     <row r="177" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A177">
-        <v>10</v>
+        <v>2.4486300999999999</v>
       </c>
       <c r="B177">
-        <v>13.566667000000001</v>
+        <v>0.70890408999999999</v>
       </c>
       <c r="C177">
-        <v>3.0999998999999998</v>
+        <v>9.6472607000000004</v>
       </c>
     </row>
     <row r="178" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A178">
-        <v>10.890351000000001</v>
+        <v>4.962707</v>
       </c>
       <c r="B178">
-        <v>6.9692983999999996</v>
+        <v>11.935082</v>
       </c>
       <c r="C178">
-        <v>12.802631</v>
+        <v>12.714088</v>
       </c>
     </row>
     <row r="179" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A179">
-        <v>3.7293389000000001</v>
+        <v>8.8255204999999997</v>
       </c>
       <c r="B179">
-        <v>8.7747936000000006</v>
+        <v>8.3619795000000003</v>
       </c>
       <c r="C179">
-        <v>12.630165</v>
+        <v>5.8489585000000002</v>
       </c>
     </row>
     <row r="180" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A180">
-        <v>0.84482758999999996</v>
+        <v>2.7107329</v>
       </c>
       <c r="B180">
-        <v>2.5086206999999998</v>
+        <v>9.5510473000000005</v>
       </c>
       <c r="C180">
-        <v>0.57758622999999998</v>
+        <v>8.6243458000000004</v>
       </c>
     </row>
     <row r="181" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A181">
-        <v>10.524448</v>
+        <v>6.8706899000000003</v>
       </c>
       <c r="B181">
-        <v>1.4629338000000001</v>
+        <v>1.1580459999999999</v>
       </c>
       <c r="C181">
-        <v>7.0843848999999999</v>
+        <v>3.8477011000000001</v>
       </c>
     </row>
     <row r="182" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A182">
-        <v>12.626238000000001</v>
+        <v>8.8728064999999994</v>
       </c>
       <c r="B182">
-        <v>2.8638612999999999</v>
+        <v>2.8201754000000001</v>
       </c>
       <c r="C182">
-        <v>9.8044557999999995</v>
+        <v>13.416667</v>
       </c>
     </row>
     <row r="183" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A183">
-        <v>13.359375</v>
+        <v>9.7870369000000004</v>
       </c>
       <c r="B183">
-        <v>6.953125</v>
+        <v>10.175926</v>
       </c>
       <c r="C183">
-        <v>0.765625</v>
+        <v>13.268518</v>
       </c>
     </row>
     <row r="184" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A184">
-        <v>1.8430233</v>
+        <v>13.08</v>
       </c>
       <c r="B184">
-        <v>1.7616278999999999</v>
+        <v>5.085</v>
       </c>
       <c r="C184">
-        <v>3.9244186999999999</v>
+        <v>1.0049999999999999</v>
       </c>
     </row>
     <row r="185" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A185">
-        <v>6.5103306999999999</v>
+        <v>7.0431032</v>
       </c>
       <c r="B185">
-        <v>6.2913221999999998</v>
+        <v>0.75</v>
       </c>
       <c r="C185">
-        <v>12.477273</v>
+        <v>9.0603446999999999</v>
       </c>
     </row>
     <row r="186" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A186">
-        <v>12.908823999999999</v>
+        <v>6.6029410000000004</v>
       </c>
       <c r="B186">
-        <v>3.7029412000000002</v>
+        <v>1.8205882</v>
       </c>
       <c r="C186">
-        <v>2.8382353999999999</v>
+        <v>1.0911765</v>
       </c>
     </row>
     <row r="187" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A187">
-        <v>11.355263000000001</v>
+        <v>8.9166670000000003</v>
       </c>
       <c r="B187">
-        <v>4.2997074</v>
+        <v>7.2333331000000003</v>
       </c>
       <c r="C187">
-        <v>9.6038008000000001</v>
+        <v>8.6166668000000008</v>
       </c>
     </row>
     <row r="188" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A188">
-        <v>0.69444441999999995</v>
+        <v>1.0323529</v>
       </c>
       <c r="B188">
-        <v>9.0138893000000007</v>
+        <v>7.1852942000000004</v>
       </c>
       <c r="C188">
-        <v>8.9722223000000003</v>
+        <v>8.5617646999999995</v>
       </c>
     </row>
     <row r="189" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A189">
-        <v>11.675703</v>
+        <v>4.9939022</v>
       </c>
       <c r="B189">
-        <v>9.0291166</v>
+        <v>13.432926999999999</v>
       </c>
       <c r="C189">
-        <v>6.629518</v>
+        <v>10.896341</v>
       </c>
     </row>
     <row r="190" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A190">
-        <v>8.0625</v>
+        <v>9.5915488999999994</v>
       </c>
       <c r="B190">
-        <v>8.8812504000000008</v>
+        <v>0.97183096000000002</v>
       </c>
       <c r="C190">
-        <v>0.95625000999999998</v>
+        <v>10.573943999999999</v>
       </c>
     </row>
     <row r="191" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A191">
-        <v>4.8155736999999998</v>
+        <v>10.476191</v>
       </c>
       <c r="B191">
-        <v>1.0204918000000001</v>
+        <v>9.9226188999999998</v>
       </c>
       <c r="C191">
-        <v>4.8073769000000004</v>
+        <v>11.458333</v>
       </c>
     </row>
     <row r="192" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A192">
-        <v>12.712365</v>
+        <v>4.9055556999999999</v>
       </c>
       <c r="B192">
-        <v>7.0349463999999999</v>
+        <v>10.638889000000001</v>
       </c>
       <c r="C192">
-        <v>4.8629030999999996</v>
+        <v>1.0277778</v>
       </c>
     </row>
     <row r="193" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A193">
-        <v>4.8739672000000001</v>
+        <v>9.6512870999999993</v>
       </c>
       <c r="B193">
-        <v>12.969008000000001</v>
+        <v>1.5075107999999999</v>
       </c>
       <c r="C193">
-        <v>7.6301651000000001</v>
+        <v>5.9581546999999997</v>
       </c>
     </row>
     <row r="194" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A194">
-        <v>0.99468082000000002</v>
+        <v>1.0733334000000001</v>
       </c>
       <c r="B194">
-        <v>2.5904254999999998</v>
+        <v>10.8</v>
       </c>
       <c r="C194">
-        <v>1.6968084999999999</v>
+        <v>12.046666999999999</v>
       </c>
     </row>
     <row r="195" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A195">
-        <v>3.75</v>
+        <v>5.5701217999999999</v>
       </c>
       <c r="B195">
-        <v>1.75</v>
+        <v>5.5914636</v>
       </c>
       <c r="C195">
-        <v>3.6458333000000001</v>
+        <v>1.7134147</v>
       </c>
     </row>
     <row r="196" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A196">
-        <v>6.1722220999999999</v>
+        <v>7.7919846000000001</v>
       </c>
       <c r="B196">
-        <v>4.1194443999999999</v>
+        <v>11.811069</v>
       </c>
       <c r="C196">
-        <v>11.316667000000001</v>
+        <v>10.818702999999999</v>
       </c>
     </row>
     <row r="197" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A197">
-        <v>3.8843283999999998</v>
+        <v>3.1333334000000002</v>
       </c>
       <c r="B197">
-        <v>1.0261194</v>
+        <v>1</v>
       </c>
       <c r="C197">
-        <v>7.2126865000000002</v>
+        <v>7.6999997999999996</v>
       </c>
     </row>
     <row r="198" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A198">
-        <v>3.5</v>
+        <v>13.284722</v>
       </c>
       <c r="B198">
-        <v>12.327586</v>
+        <v>2.7430555999999999</v>
       </c>
       <c r="C198">
-        <v>11.232759</v>
+        <v>1.6458333999999999</v>
       </c>
     </row>
     <row r="199" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A199">
-        <v>11.5</v>
+        <v>4.7408257000000003</v>
       </c>
       <c r="B199">
-        <v>13.444445</v>
+        <v>1.2362385</v>
       </c>
       <c r="C199">
-        <v>8.4722223000000003</v>
+        <v>1.0848624</v>
       </c>
     </row>
     <row r="200" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A200">
-        <v>3.25</v>
+        <v>12.655263</v>
       </c>
       <c r="B200">
-        <v>11.978724</v>
+        <v>6.6500000999999997</v>
       </c>
       <c r="C200">
-        <v>6.3882979999999998</v>
+        <v>7.8394737000000001</v>
       </c>
     </row>
     <row r="201" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A201">
-        <v>2.6721311000000001</v>
+        <v>8.7102269999999997</v>
       </c>
       <c r="B201">
-        <v>8.6311473999999997</v>
+        <v>10.681818</v>
       </c>
       <c r="C201">
-        <v>2.6926228999999999</v>
+        <v>3.5397726999999999</v>
       </c>
     </row>
     <row r="202" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A202">
-        <v>0.84589040000000004</v>
+        <v>12.031817999999999</v>
       </c>
       <c r="B202">
-        <v>1.1541096</v>
+        <v>8.7318181999999993</v>
       </c>
       <c r="C202">
-        <v>6.0650687000000003</v>
+        <v>7.7636365999999999</v>
       </c>
     </row>
     <row r="203" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A203">
-        <v>7.0025253000000003</v>
+        <v>6.5752034000000004</v>
       </c>
       <c r="B203">
-        <v>5.9015149999999998</v>
+        <v>6.5752034000000004</v>
       </c>
       <c r="C203">
-        <v>2.7904040999999999</v>
+        <v>4.1808943999999997</v>
       </c>
     </row>
     <row r="204" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A204">
-        <v>1.2398648000000001</v>
+        <v>13.266482999999999</v>
       </c>
       <c r="B204">
-        <v>6.4020270999999997</v>
+        <v>10.211537999999999</v>
       </c>
       <c r="C204">
-        <v>9.3952703</v>
+        <v>1.1785715000000001</v>
       </c>
     </row>
     <row r="205" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A205">
-        <v>4.8563828000000004</v>
+        <v>4.6285714999999996</v>
       </c>
       <c r="B205">
-        <v>0.94148933999999995</v>
+        <v>0.95714283</v>
       </c>
       <c r="C205">
-        <v>2.7074468</v>
+        <v>4.1357141000000004</v>
       </c>
     </row>
     <row r="206" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A206">
-        <v>8.75</v>
+        <v>11.118421</v>
       </c>
       <c r="B206">
-        <v>1</v>
+        <v>10.776316</v>
       </c>
       <c r="C206">
-        <v>3.1935484000000001</v>
+        <v>7.3552631999999996</v>
       </c>
     </row>
     <row r="207" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A207">
-        <v>7.2388887000000004</v>
+        <v>8.75</v>
       </c>
       <c r="B207">
-        <v>10.227777</v>
+        <v>1.4861112000000001</v>
       </c>
       <c r="C207">
-        <v>7.1166668</v>
+        <v>8.7152776999999997</v>
       </c>
     </row>
     <row r="208" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A208">
-        <v>4.8026314000000001</v>
+        <v>8.8404760000000007</v>
       </c>
       <c r="B208">
-        <v>2.6184210999999999</v>
+        <v>7.6452378999999997</v>
       </c>
       <c r="C208">
-        <v>0.69736843999999998</v>
+        <v>13.078571</v>
       </c>
     </row>
     <row r="209" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A209">
-        <v>3.6944444000000001</v>
+        <v>5.5833335000000002</v>
       </c>
       <c r="B209">
-        <v>8.6296301</v>
+        <v>5.3277779000000001</v>
       </c>
       <c r="C209">
-        <v>6.0462961000000002</v>
+        <v>4.9166664999999998</v>
       </c>
     </row>
     <row r="210" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A210">
-        <v>0.90492958000000001</v>
+        <v>10.347015000000001</v>
       </c>
       <c r="B210">
-        <v>6.7711266999999999</v>
+        <v>3.2798506999999999</v>
       </c>
       <c r="C210">
-        <v>7.0176058000000001</v>
+        <v>3.2276120000000001</v>
       </c>
     </row>
     <row r="211" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A211">
-        <v>0.77777779000000002</v>
+        <v>3.6921053000000001</v>
       </c>
       <c r="B211">
-        <v>0.95833330999999999</v>
+        <v>12.184210999999999</v>
       </c>
       <c r="C211">
-        <v>8.4027776999999997</v>
+        <v>1.4394735999999999</v>
       </c>
     </row>
     <row r="212" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A212">
-        <v>13.459301999999999</v>
+        <v>13.5625</v>
       </c>
       <c r="B212">
-        <v>3.9127907999999998</v>
+        <v>5.34375</v>
       </c>
       <c r="C212">
-        <v>12.552325</v>
+        <v>7.40625</v>
       </c>
     </row>
     <row r="213" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A213">
-        <v>0.65909094000000001</v>
+        <v>7.7362637999999997</v>
       </c>
       <c r="B213">
-        <v>5.8863634999999999</v>
+        <v>7.8434067000000001</v>
       </c>
       <c r="C213">
-        <v>3.7045455</v>
+        <v>1.7142857</v>
       </c>
     </row>
     <row r="214" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A214">
-        <v>2.6420455</v>
+        <v>12.841837</v>
       </c>
       <c r="B214">
-        <v>1.0681818999999999</v>
+        <v>7.6071429000000004</v>
       </c>
       <c r="C214">
-        <v>5.9886365000000001</v>
+        <v>0.95408165</v>
       </c>
     </row>
     <row r="215" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A215">
-        <v>7.3928570999999996</v>
+        <v>0.73333334999999999</v>
       </c>
       <c r="B215">
-        <v>13.75</v>
+        <v>12.983333999999999</v>
       </c>
       <c r="C215">
-        <v>10.535714</v>
+        <v>10.7</v>
       </c>
     </row>
     <row r="216" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A216">
-        <v>5.7906975999999997</v>
+        <v>0.98611110000000002</v>
       </c>
       <c r="B216">
-        <v>12.156976999999999</v>
+        <v>13.361110999999999</v>
       </c>
       <c r="C216">
-        <v>10.023255000000001</v>
+        <v>2.8333333000000001</v>
       </c>
     </row>
     <row r="217" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A217">
-        <v>3.4148044999999998</v>
+        <v>8.2857140999999999</v>
       </c>
       <c r="B217">
-        <v>3.0265361999999998</v>
+        <v>4.6875</v>
       </c>
       <c r="C217">
-        <v>1.6689944000000001</v>
+        <v>13.526786</v>
       </c>
     </row>
     <row r="218" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A218">
-        <v>8.1762294999999998</v>
+        <v>13.181578999999999</v>
       </c>
       <c r="B218">
-        <v>7.1598363000000003</v>
+        <v>8.8131579999999996</v>
       </c>
       <c r="C218">
-        <v>13.389343999999999</v>
+        <v>10.013158000000001</v>
       </c>
     </row>
     <row r="219" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A219">
-        <v>3.55</v>
+        <v>13.196281000000001</v>
       </c>
       <c r="B219">
-        <v>13.45</v>
+        <v>5.8119835999999996</v>
       </c>
       <c r="C219">
-        <v>13.25</v>
+        <v>10.840909</v>
       </c>
     </row>
     <row r="220" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A220">
-        <v>5.0605263999999996</v>
+        <v>8.336957</v>
       </c>
       <c r="B220">
-        <v>1.3131579</v>
+        <v>1.7355072</v>
       </c>
       <c r="C220">
-        <v>9.2657889999999998</v>
+        <v>0.91666669000000001</v>
       </c>
     </row>
     <row r="221" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A221">
-        <v>12.8</v>
+        <v>0.89705884000000002</v>
       </c>
       <c r="B221">
-        <v>11.5</v>
+        <v>3.7058822999999999</v>
       </c>
       <c r="C221">
-        <v>8.9499998000000005</v>
+        <v>11.992647</v>
       </c>
     </row>
     <row r="222" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A222">
-        <v>4.9499997999999996</v>
+        <v>3.6117021999999999</v>
       </c>
       <c r="B222">
-        <v>7.7420001000000003</v>
+        <v>6.7287235000000001</v>
       </c>
       <c r="C222">
-        <v>10.762</v>
+        <v>3.5691489999999999</v>
       </c>
     </row>
     <row r="223" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A223">
-        <v>0.96739131</v>
+        <v>1.0792683000000001</v>
       </c>
       <c r="B223">
-        <v>13.315217000000001</v>
+        <v>1.1371951</v>
       </c>
       <c r="C223">
-        <v>9.9456520000000008</v>
+        <v>7.1128049000000004</v>
       </c>
     </row>
     <row r="224" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A224">
-        <v>8.0588236000000002</v>
+        <v>11.564569000000001</v>
       </c>
       <c r="B224">
-        <v>13.485294</v>
+        <v>7.8592715000000002</v>
       </c>
       <c r="C224">
-        <v>5.4705881999999999</v>
+        <v>12.922186</v>
       </c>
     </row>
     <row r="225" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A225">
-        <v>10.75</v>
+        <v>12.585526</v>
       </c>
       <c r="B225">
-        <v>0.58333330999999999</v>
+        <v>4.6743421999999999</v>
       </c>
       <c r="C225">
-        <v>7.9166664999999998</v>
+        <v>3.5460527000000002</v>
       </c>
     </row>
     <row r="226" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A226">
-        <v>11.556666</v>
+        <v>10.715909</v>
       </c>
       <c r="B226">
-        <v>3.2366666999999998</v>
+        <v>9.8143940000000001</v>
       </c>
       <c r="C226">
-        <v>13.106667</v>
+        <v>9.1856059999999999</v>
       </c>
     </row>
     <row r="227" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A227">
-        <v>9.8839283000000009</v>
+        <v>10.717105</v>
       </c>
       <c r="B227">
-        <v>4.6607140999999999</v>
+        <v>5.8684210999999999</v>
       </c>
       <c r="C227">
-        <v>7.0178570999999996</v>
+        <v>7.7763156999999996</v>
       </c>
     </row>
     <row r="228" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A228">
-        <v>1.0523256000000001</v>
+        <v>7.0833335000000002</v>
       </c>
       <c r="B228">
-        <v>13.30814</v>
+        <v>12.592592</v>
       </c>
       <c r="C228">
-        <v>3.1337209000000001</v>
+        <v>7.2962961000000002</v>
       </c>
     </row>
     <row r="229" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A229">
-        <v>13.35</v>
+        <v>3.9076086999999999</v>
       </c>
       <c r="B229">
-        <v>8.7388887000000004</v>
+        <v>1.0652174000000001</v>
       </c>
       <c r="C229">
-        <v>1.1277778000000001</v>
+        <v>12.744565</v>
       </c>
     </row>
     <row r="230" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A230">
-        <v>1.4732143</v>
+        <v>12.047794</v>
       </c>
       <c r="B230">
-        <v>1.1041666000000001</v>
+        <v>4.4301472000000004</v>
       </c>
       <c r="C230">
-        <v>12.497024</v>
+        <v>13.202206</v>
       </c>
     </row>
     <row r="231" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A231">
-        <v>8.7150353999999997</v>
+        <v>9.1184206000000003</v>
       </c>
       <c r="B231">
-        <v>3.0087410999999999</v>
+        <v>11.969298</v>
       </c>
       <c r="C231">
-        <v>8.1066436999999993</v>
+        <v>8.2149123999999993</v>
       </c>
     </row>
     <row r="232" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A232">
-        <v>8.8206520000000008</v>
+        <v>13.625</v>
       </c>
       <c r="B232">
-        <v>1.0380434999999999</v>
+        <v>3.7083333000000001</v>
       </c>
       <c r="C232">
-        <v>12.847826</v>
+        <v>5.1666664999999998</v>
       </c>
     </row>
     <row r="233" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A233">
-        <v>10.928572000000001</v>
+        <v>1.4059139</v>
       </c>
       <c r="B233">
-        <v>6.7857140999999999</v>
+        <v>1.3413979</v>
       </c>
       <c r="C233">
-        <v>1.2142857</v>
+        <v>13.303763</v>
       </c>
     </row>
     <row r="234" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A234">
-        <v>10.818182</v>
+        <v>8.75</v>
       </c>
       <c r="B234">
-        <v>11.068182</v>
+        <v>13</v>
       </c>
       <c r="C234">
-        <v>2.6136363</v>
+        <v>13.75</v>
       </c>
     </row>
     <row r="235" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A235">
-        <v>5.9541801999999997</v>
+        <v>6.4545455</v>
       </c>
       <c r="B235">
-        <v>11.753216</v>
+        <v>3.5</v>
       </c>
       <c r="C235">
-        <v>4.7001609999999996</v>
+        <v>0.84090905999999999</v>
       </c>
     </row>
     <row r="236" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A236">
-        <v>12.942307</v>
+        <v>3.5707548</v>
       </c>
       <c r="B236">
-        <v>13.365385</v>
+        <v>8.7169808999999994</v>
       </c>
       <c r="C236">
-        <v>8.3846149000000008</v>
+        <v>3.7028300999999999</v>
       </c>
     </row>
     <row r="237" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A237">
-        <v>4.2376031999999997</v>
+        <v>13.544117999999999</v>
       </c>
       <c r="B237">
-        <v>5.0516528999999997</v>
+        <v>3.6911763999999998</v>
       </c>
       <c r="C237">
-        <v>2.9524794000000001</v>
+        <v>8.5147057000000004</v>
       </c>
     </row>
     <row r="238" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A238">
-        <v>6.6810346000000003</v>
+        <v>10.558332999999999</v>
       </c>
       <c r="B238">
-        <v>7.6637931000000004</v>
+        <v>4.8249997999999996</v>
       </c>
       <c r="C238">
-        <v>7.8534484000000004</v>
+        <v>6.6500000999999997</v>
       </c>
     </row>
     <row r="239" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A239">
-        <v>2.1757426</v>
+        <v>13.201219999999999</v>
       </c>
       <c r="B239">
-        <v>10.284654</v>
+        <v>0.84756100000000001</v>
       </c>
       <c r="C239">
-        <v>12.923266999999999</v>
+        <v>1.6280488</v>
       </c>
     </row>
     <row r="240" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A240">
-        <v>6.8529963</v>
+        <v>6.2874999000000003</v>
       </c>
       <c r="B240">
-        <v>12.712546</v>
+        <v>12.887499999999999</v>
       </c>
       <c r="C240">
-        <v>1.5121723</v>
+        <v>2.9708332999999998</v>
       </c>
     </row>
     <row r="241" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A241">
-        <v>1.8780992000000001</v>
+        <v>13.108025</v>
       </c>
       <c r="B241">
-        <v>13.13843</v>
+        <v>7.5709876999999999</v>
       </c>
       <c r="C241">
-        <v>8.0309916000000001</v>
+        <v>2.6697530999999999</v>
       </c>
     </row>
     <row r="242" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A242">
-        <v>10.516666000000001</v>
+        <v>0.64999998000000003</v>
       </c>
       <c r="B242">
-        <v>10.961111000000001</v>
+        <v>13.55</v>
       </c>
       <c r="C242">
-        <v>0.85000001999999997</v>
+        <v>13.5</v>
       </c>
     </row>
     <row r="243" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A243">
-        <v>11.384831</v>
+        <v>4.9780702999999997</v>
       </c>
       <c r="B243">
-        <v>13.047751999999999</v>
+        <v>3.8552632</v>
       </c>
       <c r="C243">
-        <v>1.1376405000000001</v>
+        <v>9.8815793999999997</v>
       </c>
     </row>
     <row r="244" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A244">
-        <v>4.9230771000000004</v>
+        <v>7.8131069999999996</v>
       </c>
       <c r="B244">
-        <v>10.576923000000001</v>
+        <v>10.691748</v>
       </c>
       <c r="C244">
-        <v>1.8115384999999999</v>
+        <v>1.1286408000000001</v>
       </c>
     </row>
     <row r="245" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A245">
-        <v>7.0604576999999997</v>
+        <v>8.8284310999999995</v>
       </c>
       <c r="B245">
-        <v>2.8316994000000002</v>
+        <v>10.936275</v>
       </c>
       <c r="C245">
-        <v>5.6977124000000003</v>
+        <v>5.2107843999999996</v>
       </c>
     </row>
     <row r="246" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A246">
-        <v>3.3157895000000002</v>
+        <v>10.726744999999999</v>
       </c>
       <c r="B246">
-        <v>12.9375</v>
+        <v>12.093023000000001</v>
       </c>
       <c r="C246">
-        <v>4.2368421999999999</v>
+        <v>2.9767442000000002</v>
       </c>
     </row>
     <row r="247" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A247">
-        <v>12.629630000000001</v>
+        <v>1.1722223000000001</v>
       </c>
       <c r="B247">
-        <v>5.7222223000000003</v>
+        <v>7.0611110000000004</v>
       </c>
       <c r="C247">
-        <v>13.351851</v>
+        <v>10.438889</v>
       </c>
     </row>
     <row r="248" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A248">
-        <v>3.9342104999999998</v>
+        <v>6.5637255000000003</v>
       </c>
       <c r="B248">
-        <v>2.9342104999999998</v>
+        <v>12.828431</v>
       </c>
       <c r="C248">
-        <v>10.888158000000001</v>
+        <v>0.92647058000000004</v>
       </c>
     </row>
     <row r="249" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A249">
-        <v>12.668919000000001</v>
+        <v>4.6691918000000001</v>
       </c>
       <c r="B249">
-        <v>6.8445945000000004</v>
+        <v>3.7904040999999999</v>
       </c>
       <c r="C249">
-        <v>2.4121621000000002</v>
+        <v>13.270201999999999</v>
       </c>
     </row>
     <row r="250" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A250">
-        <v>13.409091</v>
+        <v>11.863636</v>
       </c>
       <c r="B250">
-        <v>13.431818</v>
+        <v>13.522727</v>
       </c>
       <c r="C250">
-        <v>1.3863635999999999</v>
+        <v>4.2045455</v>
       </c>
     </row>
     <row r="251" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A251">
-        <v>3.45</v>
+        <v>11.304688000000001</v>
       </c>
       <c r="B251">
-        <v>10.75</v>
+        <v>8.4765625</v>
       </c>
       <c r="C251">
-        <v>9.8973683999999995</v>
+        <v>5.9140625</v>
       </c>
     </row>
     <row r="252" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A252">
-        <v>12.618421</v>
+        <v>0.92424244</v>
       </c>
       <c r="B252">
-        <v>0.67105263000000004</v>
+        <v>5.4318179999999998</v>
       </c>
       <c r="C252">
-        <v>6.2763156999999996</v>
+        <v>0.73484850000000002</v>
       </c>
     </row>
     <row r="253" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A253">
-        <v>8.4659767000000006</v>
+        <v>3.048969</v>
       </c>
       <c r="B253">
-        <v>10.960058999999999</v>
+        <v>2.6829896</v>
       </c>
       <c r="C253">
-        <v>12.386094999999999</v>
+        <v>10.136597999999999</v>
       </c>
     </row>
     <row r="254" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A254">
-        <v>1.0727848</v>
+        <v>2</v>
       </c>
       <c r="B254">
-        <v>8.2689877000000003</v>
+        <v>4.3375000999999997</v>
       </c>
       <c r="C254">
-        <v>10.946202</v>
+        <v>6.9562502000000004</v>
       </c>
     </row>
   </sheetData>
@@ -4045,18 +4045,18 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
   <Edit>DocumentLibraryForm</Edit>
   <New>DocumentLibraryForm</New>
 </FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
@@ -4263,18 +4263,18 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{84B75DF6-E9B7-46AF-A237-716DDC59A331}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3BF7FACE-1743-4185-A432-BBDBC75AE110}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3BF7FACE-1743-4185-A432-BBDBC75AE110}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{84B75DF6-E9B7-46AF-A237-716DDC59A331}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>

<commit_message>
added an additional dependence on distance from grain boundary
</commit_message>
<xml_diff>
--- a/Dream3d2Abaqus/inputfile_info.xlsx
+++ b/Dream3d2Abaqus/inputfile_info.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mi19356\OneDrive - University of Bristol\Documents\CP_simulations\Dream3d2Abaqus\Dream3d2Abaqus\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="16" documentId="8_{B136ABAE-EB51-4A80-BA81-9E123800CD73}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{DD30ADD4-E938-434D-98EA-BC9D9461AF90}"/>
+  <xr:revisionPtr revIDLastSave="4" documentId="114_{F53572BA-BA47-49EE-9FCA-A4278B2FE462}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{FED13CF5-0C86-4874-B69E-E041CF6A3D44}"/>
   <bookViews>
-    <workbookView xWindow="380" yWindow="380" windowWidth="13880" windowHeight="9190" xr2:uid="{B2FFBA9E-8DF3-44DC-8BFA-5D5291E16B1C}"/>
+    <workbookView xWindow="5410" yWindow="1180" windowWidth="13880" windowHeight="9190" activeTab="1" xr2:uid="{B2FFBA9E-8DF3-44DC-8BFA-5D5291E16B1C}"/>
   </bookViews>
   <sheets>
     <sheet name="Material_parameters" sheetId="1" r:id="rId1"/>
@@ -382,8 +382,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0A2FF6DC-890B-49C6-8880-6BB58835CE0B}">
   <dimension ref="A1:A168"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A166" sqref="A166"/>
+    <sheetView topLeftCell="A91" workbookViewId="0">
+      <selection activeCell="B99" sqref="B99"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -870,17 +870,17 @@
     </row>
     <row r="97" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A97">
-        <v>100</v>
+        <v>50</v>
       </c>
     </row>
     <row r="98" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A98">
-        <v>190</v>
+        <v>50</v>
       </c>
     </row>
     <row r="99" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A99">
-        <v>280</v>
+        <v>100</v>
       </c>
     </row>
     <row r="100" spans="1:1" x14ac:dyDescent="0.35">
@@ -1236,2806 +1236,1827 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C8E9C165-EF39-4A1B-9ECE-A782E2B0DD1A}">
-  <dimension ref="A1:C254"/>
+  <dimension ref="A1:C165"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:C254"/>
+    <sheetView tabSelected="1" topLeftCell="A160" workbookViewId="0">
+      <selection sqref="A1:C165"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A1">
-        <v>9.0500001999999995</v>
+        <v>5.186007</v>
       </c>
       <c r="B1">
-        <v>3.6500001000000002</v>
+        <v>16.097269000000001</v>
       </c>
       <c r="C1">
-        <v>1.8571428000000001</v>
+        <v>2.7627985000000002</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A2">
-        <v>3.8646498</v>
+        <v>2.7361702999999999</v>
       </c>
       <c r="B2">
-        <v>1.7277070000000001</v>
+        <v>6.1170210999999997</v>
       </c>
       <c r="C2">
-        <v>5.9570065000000003</v>
+        <v>22.055319000000001</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A3">
-        <v>7.75</v>
+        <v>37.600558999999997</v>
       </c>
       <c r="B3">
-        <v>10.75</v>
+        <v>8.2094974999999994</v>
       </c>
       <c r="C3">
-        <v>0.75</v>
+        <v>27.885475</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A4">
-        <v>5.6829267000000003</v>
+        <v>36.391689</v>
       </c>
       <c r="B4">
-        <v>8.8414631000000004</v>
+        <v>20.323677</v>
       </c>
       <c r="C4">
-        <v>4.9268292999999996</v>
+        <v>21.074306</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A5">
-        <v>3.8622448</v>
+        <v>8.7435483999999999</v>
       </c>
       <c r="B5">
-        <v>9.7857140999999999</v>
+        <v>24.729033000000001</v>
       </c>
       <c r="C5">
-        <v>1.9591837000000001</v>
+        <v>6.8064517999999996</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A6">
-        <v>11.643617000000001</v>
+        <v>37.161617</v>
       </c>
       <c r="B6">
-        <v>13.579787</v>
+        <v>14.651515</v>
       </c>
       <c r="C6">
-        <v>13.079787</v>
+        <v>2.8535354000000002</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A7">
-        <v>2.0614754999999998</v>
+        <v>34.916446999999998</v>
       </c>
       <c r="B7">
-        <v>3.1926228999999999</v>
+        <v>5.5106101000000001</v>
       </c>
       <c r="C7">
-        <v>3.8073771000000001</v>
+        <v>36.868701999999999</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A8">
-        <v>7.3235292000000003</v>
+        <v>4.4425739999999996</v>
       </c>
       <c r="B8">
-        <v>1.5</v>
+        <v>3.1970296</v>
       </c>
       <c r="C8">
-        <v>11.595589</v>
+        <v>35.923763000000001</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A9">
-        <v>13.22541</v>
+        <v>30.401185999999999</v>
       </c>
       <c r="B9">
-        <v>10.70082</v>
+        <v>33.009880000000003</v>
       </c>
       <c r="C9">
-        <v>12.151638999999999</v>
+        <v>18.211462000000001</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A10">
-        <v>11.766949</v>
+        <v>31.025691999999999</v>
       </c>
       <c r="B10">
-        <v>1.1483051</v>
+        <v>18.835968000000001</v>
       </c>
       <c r="C10">
-        <v>3.0805085000000001</v>
+        <v>2.5474307999999999</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A11">
-        <v>13.385135</v>
+        <v>3.7702703</v>
       </c>
       <c r="B11">
-        <v>7.2364864000000004</v>
+        <v>34.193694999999998</v>
       </c>
       <c r="C11">
-        <v>6.6554054999999996</v>
+        <v>33.6021</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A12">
-        <v>7.3666668</v>
+        <v>3.6191765999999999</v>
       </c>
       <c r="B12">
-        <v>11.3</v>
+        <v>19.770856999999999</v>
       </c>
       <c r="C12">
-        <v>8.7666664000000001</v>
+        <v>26.787106999999999</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A13">
-        <v>3.6083333</v>
+        <v>19.791924999999999</v>
       </c>
       <c r="B13">
-        <v>12.083333</v>
+        <v>13.723602</v>
       </c>
       <c r="C13">
-        <v>11.333333</v>
+        <v>21.493790000000001</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A14">
-        <v>11.958955</v>
+        <v>23.126864999999999</v>
       </c>
       <c r="B14">
-        <v>12.160448000000001</v>
+        <v>16.328358000000001</v>
       </c>
       <c r="C14">
-        <v>0.94029850000000004</v>
+        <v>38.358207999999998</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A15">
-        <v>2.0592104999999998</v>
+        <v>32.200854999999997</v>
       </c>
       <c r="B15">
-        <v>10.118421</v>
+        <v>38.217948999999997</v>
       </c>
       <c r="C15">
-        <v>3.7302632</v>
+        <v>3.2820513</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A16">
-        <v>13.356061</v>
+        <v>22.080393000000001</v>
       </c>
       <c r="B16">
-        <v>5.6439395000000001</v>
+        <v>23.103922000000001</v>
       </c>
       <c r="C16">
-        <v>8.8409089999999999</v>
+        <v>19.907843</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A17">
-        <v>0.97093021999999995</v>
+        <v>10.309917</v>
       </c>
       <c r="B17">
-        <v>7.6337209000000001</v>
+        <v>23.380991000000002</v>
       </c>
       <c r="C17">
-        <v>3.5872092000000002</v>
+        <v>19.605785000000001</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A18">
-        <v>2.9619564999999999</v>
+        <v>7.7815532999999997</v>
       </c>
       <c r="B18">
-        <v>5.9728260000000004</v>
+        <v>27.485437000000001</v>
       </c>
       <c r="C18">
-        <v>0.97826086999999995</v>
+        <v>35.893203999999997</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A19">
-        <v>13.460526</v>
+        <v>17.591145999999998</v>
       </c>
       <c r="B19">
-        <v>1.1184210999999999</v>
+        <v>13.492188000000001</v>
       </c>
       <c r="C19">
-        <v>11.881579</v>
+        <v>2.828125</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A20">
-        <v>8.3790320999999999</v>
+        <v>13.221705999999999</v>
       </c>
       <c r="B20">
-        <v>3.7951611999999999</v>
+        <v>20.620594000000001</v>
       </c>
       <c r="C20">
-        <v>4.5016131000000001</v>
+        <v>9.8543596000000004</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A21">
-        <v>11.603659</v>
+        <v>37.864638999999997</v>
       </c>
       <c r="B21">
-        <v>4.0060978</v>
+        <v>5.8701657999999997</v>
       </c>
       <c r="C21">
-        <v>10.908537000000001</v>
+        <v>2.0303867000000002</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A22">
-        <v>9.0219296999999994</v>
+        <v>8.3235291999999994</v>
       </c>
       <c r="B22">
-        <v>1.0657894999999999</v>
+        <v>14.626697</v>
       </c>
       <c r="C22">
-        <v>2.9868421999999999</v>
+        <v>29.880091</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A23">
-        <v>6.7688680000000003</v>
+        <v>37.973331000000002</v>
       </c>
       <c r="B23">
-        <v>12.75</v>
+        <v>20.5</v>
       </c>
       <c r="C23">
-        <v>12.627357999999999</v>
+        <v>2.6666666999999999</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A24">
-        <v>11.807693</v>
+        <v>36.665241000000002</v>
       </c>
       <c r="B24">
-        <v>6.7692307999999999</v>
+        <v>3.4544160000000002</v>
       </c>
       <c r="C24">
-        <v>1</v>
+        <v>12.405983000000001</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A25">
-        <v>3.7039472999999998</v>
+        <v>32.868133999999998</v>
       </c>
       <c r="B25">
-        <v>8.2105265000000003</v>
+        <v>12.021978000000001</v>
       </c>
       <c r="C25">
-        <v>11.302631</v>
+        <v>2.5824175</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A26">
-        <v>0.87</v>
+        <v>36.848880999999999</v>
       </c>
       <c r="B26">
-        <v>6.9299998</v>
+        <v>29.020523000000001</v>
       </c>
       <c r="C26">
-        <v>2.0799998999999998</v>
+        <v>21.098880999999999</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A27">
-        <v>13.544117999999999</v>
+        <v>36.393856</v>
       </c>
       <c r="B27">
-        <v>13.632353</v>
+        <v>28.086592</v>
       </c>
       <c r="C27">
-        <v>10.044117999999999</v>
+        <v>30.844507</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A28">
-        <v>10.645833</v>
+        <v>14.828918</v>
       </c>
       <c r="B28">
-        <v>7.7708335000000002</v>
+        <v>9.7097130000000007</v>
       </c>
       <c r="C28">
-        <v>8.7708329999999997</v>
+        <v>8.9591607999999994</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A29">
-        <v>1.2470238</v>
+        <v>35.519607999999998</v>
       </c>
       <c r="B29">
-        <v>8.0982140999999999</v>
+        <v>37.377006999999999</v>
       </c>
       <c r="C29">
-        <v>12.464286</v>
+        <v>23.863636</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A30">
-        <v>9.9866075999999993</v>
+        <v>17.942785000000001</v>
       </c>
       <c r="B30">
-        <v>6.7901787999999996</v>
+        <v>33.310943999999999</v>
       </c>
       <c r="C30">
-        <v>2.9285714999999999</v>
+        <v>2.8233831</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A31">
-        <v>4.6071429000000004</v>
+        <v>21.285276</v>
       </c>
       <c r="B31">
-        <v>9.3928575999999993</v>
+        <v>8.1012267999999992</v>
       </c>
       <c r="C31">
-        <v>2.8928571000000001</v>
+        <v>30.107362999999999</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A32">
-        <v>11.626811999999999</v>
+        <v>10.931452</v>
       </c>
       <c r="B32">
-        <v>8.786232</v>
+        <v>7.7137098000000002</v>
       </c>
       <c r="C32">
-        <v>1.134058</v>
+        <v>36.514113999999999</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A33">
-        <v>10.771739</v>
+        <v>29.478494999999999</v>
       </c>
       <c r="B33">
-        <v>9.3079710000000002</v>
+        <v>15.515639999999999</v>
       </c>
       <c r="C33">
-        <v>3.6775362</v>
+        <v>10.606548999999999</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A34">
-        <v>6.4819589000000004</v>
+        <v>10.36755</v>
       </c>
       <c r="B34">
-        <v>11.507732000000001</v>
+        <v>19.447019999999998</v>
       </c>
       <c r="C34">
-        <v>3.9201031</v>
+        <v>25.586092000000001</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A35">
-        <v>0.91666669000000001</v>
+        <v>20.927481</v>
       </c>
       <c r="B35">
-        <v>5.3194447</v>
+        <v>26.003817000000002</v>
       </c>
       <c r="C35">
-        <v>8.5694447</v>
+        <v>30.782442</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A36">
-        <v>8.9523811000000002</v>
+        <v>2.6214057999999998</v>
       </c>
       <c r="B36">
-        <v>0.75</v>
+        <v>32.531948</v>
       </c>
       <c r="C36">
-        <v>1.4761903999999999</v>
+        <v>13.602237000000001</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A37">
-        <v>1</v>
+        <v>14.164255000000001</v>
       </c>
       <c r="B37">
-        <v>5.75</v>
+        <v>16.016642000000001</v>
       </c>
       <c r="C37">
-        <v>11.678572000000001</v>
+        <v>35.717075000000001</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A38">
-        <v>3.5789472999999998</v>
+        <v>14.822751</v>
       </c>
       <c r="B38">
-        <v>5.9835525000000001</v>
+        <v>1.8756614</v>
       </c>
       <c r="C38">
-        <v>8.8256578000000001</v>
+        <v>31.653438999999999</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A39">
-        <v>6.6808943999999997</v>
+        <v>2.7634921000000001</v>
       </c>
       <c r="B39">
-        <v>10.046747999999999</v>
+        <v>2.8904762000000002</v>
       </c>
       <c r="C39">
-        <v>6.1117887</v>
+        <v>13.541270000000001</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A40">
-        <v>9.9642859000000001</v>
+        <v>3.5545453999999999</v>
       </c>
       <c r="B40">
-        <v>13.292857</v>
+        <v>21.639395</v>
       </c>
       <c r="C40">
-        <v>0.59285712000000002</v>
+        <v>11.360606000000001</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A41">
-        <v>5.7800001999999999</v>
+        <v>38.025345000000002</v>
       </c>
       <c r="B41">
-        <v>5.4499997999999996</v>
+        <v>36.983871000000001</v>
       </c>
       <c r="C41">
-        <v>7.02</v>
+        <v>4.9423962000000001</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A42">
-        <v>1.0714284999999999</v>
+        <v>9.8333329999999997</v>
       </c>
       <c r="B42">
-        <v>3.7559524</v>
+        <v>9.9679488999999997</v>
       </c>
       <c r="C42">
-        <v>1.6547619</v>
+        <v>2.4423077000000002</v>
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A43">
-        <v>11.675000000000001</v>
+        <v>2.6243522000000001</v>
       </c>
       <c r="B43">
-        <v>12.05</v>
+        <v>2.1476684000000001</v>
       </c>
       <c r="C43">
-        <v>5.4499997999999996</v>
+        <v>5.3445596999999996</v>
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A44">
-        <v>6.0416664999999998</v>
+        <v>19.896312999999999</v>
       </c>
       <c r="B44">
-        <v>4</v>
+        <v>37.241936000000003</v>
       </c>
       <c r="C44">
-        <v>6.4583335000000002</v>
+        <v>7.7672810999999999</v>
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A45">
-        <v>3.6931818000000001</v>
+        <v>23.939394</v>
       </c>
       <c r="B45">
-        <v>4.8352275000000002</v>
+        <v>3.7848484999999998</v>
       </c>
       <c r="C45">
-        <v>2.8409089999999999</v>
+        <v>34.239395000000002</v>
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A46">
-        <v>2.578125</v>
+        <v>1.9845360999999999</v>
       </c>
       <c r="B46">
-        <v>13.429688000000001</v>
+        <v>9.7886600000000001</v>
       </c>
       <c r="C46">
-        <v>7.0703125</v>
+        <v>8.7061852999999996</v>
       </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A47">
-        <v>7.7989511</v>
+        <v>19.515837000000001</v>
       </c>
       <c r="B47">
-        <v>4.7604895000000003</v>
+        <v>9.6968326999999999</v>
       </c>
       <c r="C47">
-        <v>1.2185315000000001</v>
+        <v>36.054298000000003</v>
       </c>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A48">
-        <v>4.7094592999999998</v>
+        <v>38.752102000000001</v>
       </c>
       <c r="B48">
-        <v>1.7837837999999999</v>
+        <v>24.079832</v>
       </c>
       <c r="C48">
-        <v>9.7297297</v>
+        <v>13.592437</v>
       </c>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A49">
-        <v>5.4625000999999997</v>
+        <v>19.831491</v>
       </c>
       <c r="B49">
-        <v>13.4</v>
+        <v>28.174032</v>
       </c>
       <c r="C49">
-        <v>7.4250002000000004</v>
+        <v>9.9033145999999999</v>
       </c>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A50">
-        <v>1.0107143000000001</v>
+        <v>19.692592999999999</v>
       </c>
       <c r="B50">
-        <v>9.0428572000000003</v>
+        <v>36.848148000000002</v>
       </c>
       <c r="C50">
-        <v>1.2071428</v>
+        <v>37.922221999999998</v>
       </c>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A51">
-        <v>13.018966000000001</v>
+        <v>9.3925619000000005</v>
       </c>
       <c r="B51">
-        <v>1.587931</v>
+        <v>2.2933884</v>
       </c>
       <c r="C51">
-        <v>5.8844829000000001</v>
+        <v>9.4256200999999997</v>
       </c>
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A52">
-        <v>0.89285713</v>
+        <v>7.3792453</v>
       </c>
       <c r="B52">
-        <v>5.8928570999999996</v>
+        <v>7.1377357999999997</v>
       </c>
       <c r="C52">
-        <v>13.535714</v>
+        <v>7.9377360000000001</v>
       </c>
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A53">
-        <v>9.6163367999999991</v>
+        <v>27.177084000000001</v>
       </c>
       <c r="B53">
-        <v>6.9628711000000001</v>
+        <v>3.6319444000000001</v>
       </c>
       <c r="C53">
-        <v>0.90841585000000002</v>
+        <v>25.916665999999999</v>
       </c>
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A54">
-        <v>13.357142</v>
+        <v>21.988987000000002</v>
       </c>
       <c r="B54">
-        <v>13.160714</v>
+        <v>35.808368999999999</v>
       </c>
       <c r="C54">
-        <v>2.0625</v>
+        <v>26.411894</v>
       </c>
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A55">
-        <v>0.93333334000000001</v>
+        <v>25.099502999999999</v>
       </c>
       <c r="B55">
-        <v>5.8333335000000002</v>
+        <v>22.905472</v>
       </c>
       <c r="C55">
-        <v>12.616667</v>
+        <v>15.266170000000001</v>
       </c>
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A56">
-        <v>11.638158000000001</v>
+        <v>2.4008620000000001</v>
       </c>
       <c r="B56">
-        <v>0.98026316999999996</v>
+        <v>17.883621000000002</v>
       </c>
       <c r="C56">
-        <v>0.67105263000000004</v>
+        <v>7.7155170000000002</v>
       </c>
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A57">
-        <v>1.7971698</v>
+        <v>37.094807000000003</v>
       </c>
       <c r="B57">
-        <v>12.858491000000001</v>
+        <v>12.162337000000001</v>
       </c>
       <c r="C57">
-        <v>13.018867</v>
+        <v>35.806491999999999</v>
       </c>
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A58">
-        <v>12.453882999999999</v>
+        <v>7.9348893</v>
       </c>
       <c r="B58">
-        <v>13.415049</v>
+        <v>3.0454545</v>
       </c>
       <c r="C58">
-        <v>6.6868930000000004</v>
+        <v>27.539311999999999</v>
       </c>
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A59">
-        <v>9.4565219999999997</v>
+        <v>28.967533</v>
       </c>
       <c r="B59">
-        <v>2.0869564999999999</v>
+        <v>11.211039</v>
       </c>
       <c r="C59">
-        <v>12.260870000000001</v>
+        <v>33.993507000000001</v>
       </c>
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A60">
-        <v>10.416667</v>
+        <v>13.841074000000001</v>
       </c>
       <c r="B60">
-        <v>5.8148150000000003</v>
+        <v>4.2300433999999996</v>
       </c>
       <c r="C60">
-        <v>11.342592</v>
+        <v>3.1008708</v>
       </c>
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A61">
-        <v>5.6434913</v>
+        <v>21.966332999999999</v>
       </c>
       <c r="B61">
-        <v>12.738166</v>
+        <v>22.342894000000001</v>
       </c>
       <c r="C61">
-        <v>5.5428996000000001</v>
+        <v>35.931423000000002</v>
       </c>
     </row>
     <row r="62" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A62">
-        <v>5.8543953999999996</v>
+        <v>12.813725</v>
       </c>
       <c r="B62">
-        <v>8.8269234000000001</v>
+        <v>20.941177</v>
       </c>
       <c r="C62">
-        <v>12.486262999999999</v>
+        <v>2.3039215</v>
       </c>
     </row>
     <row r="63" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A63">
-        <v>8.5654763999999997</v>
+        <v>19.475266000000001</v>
       </c>
       <c r="B63">
-        <v>9.7857140999999999</v>
+        <v>21.461130000000001</v>
       </c>
       <c r="C63">
-        <v>8.7261906000000007</v>
+        <v>3.9346290000000002</v>
       </c>
     </row>
     <row r="64" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A64">
-        <v>9.8697920000000003</v>
+        <v>24.770161000000002</v>
       </c>
       <c r="B64">
-        <v>3.8541666999999999</v>
+        <v>34.193550000000002</v>
       </c>
       <c r="C64">
-        <v>11.770833</v>
+        <v>2.8185484000000001</v>
       </c>
     </row>
     <row r="65" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A65">
-        <v>1.0184211000000001</v>
+        <v>13.412281</v>
       </c>
       <c r="B65">
-        <v>8.8868417999999991</v>
+        <v>33.456139</v>
       </c>
       <c r="C65">
-        <v>5.3184208999999996</v>
+        <v>25.061402999999999</v>
       </c>
     </row>
     <row r="66" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A66">
-        <v>1.9237287999999999</v>
+        <v>14.568099999999999</v>
       </c>
       <c r="B66">
-        <v>12.508474</v>
+        <v>11.688172</v>
       </c>
       <c r="C66">
-        <v>2.0677967000000002</v>
+        <v>26.630825000000002</v>
       </c>
     </row>
     <row r="67" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A67">
-        <v>12.552469</v>
+        <v>17.614906000000001</v>
       </c>
       <c r="B67">
-        <v>1.0895060999999999</v>
+        <v>27.422359</v>
       </c>
       <c r="C67">
-        <v>9.7901229999999995</v>
+        <v>35.748446999999999</v>
       </c>
     </row>
     <row r="68" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A68">
-        <v>6.9433961000000002</v>
+        <v>24.823353000000001</v>
       </c>
       <c r="B68">
-        <v>0.86320752000000001</v>
+        <v>30.098803</v>
       </c>
       <c r="C68">
-        <v>6.75</v>
+        <v>20.284431000000001</v>
       </c>
     </row>
     <row r="69" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A69">
-        <v>7.9277778000000003</v>
+        <v>23.560226</v>
       </c>
       <c r="B69">
-        <v>4.9277778000000003</v>
+        <v>36.735225999999997</v>
       </c>
       <c r="C69">
-        <v>11.775926</v>
+        <v>16.542045999999999</v>
       </c>
     </row>
     <row r="70" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A70">
-        <v>3.45</v>
+        <v>13.772402</v>
       </c>
       <c r="B70">
-        <v>12.676087000000001</v>
+        <v>26.012544999999999</v>
       </c>
       <c r="C70">
-        <v>4.8369565000000003</v>
+        <v>2.4964159000000001</v>
       </c>
     </row>
     <row r="71" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A71">
-        <v>6.6136365000000001</v>
+        <v>19.590047999999999</v>
       </c>
       <c r="B71">
-        <v>4.8409089999999999</v>
+        <v>23.196681999999999</v>
       </c>
       <c r="C71">
-        <v>2.8863637</v>
+        <v>12.779621000000001</v>
       </c>
     </row>
     <row r="72" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A72">
-        <v>12.599463</v>
+        <v>15.786407000000001</v>
       </c>
       <c r="B72">
-        <v>1.2123656</v>
+        <v>6.2912621</v>
       </c>
       <c r="C72">
-        <v>13.067204</v>
+        <v>30.106795999999999</v>
       </c>
     </row>
     <row r="73" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A73">
-        <v>6.7785716000000003</v>
+        <v>29.964441000000001</v>
       </c>
       <c r="B73">
-        <v>2.7714286000000001</v>
+        <v>36.677067000000001</v>
       </c>
       <c r="C73">
-        <v>6.7928572000000003</v>
+        <v>35.029755000000002</v>
       </c>
     </row>
     <row r="74" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A74">
-        <v>4.7790698999999996</v>
+        <v>21.834021</v>
       </c>
       <c r="B74">
-        <v>7.8313950999999999</v>
+        <v>27.592783000000001</v>
       </c>
       <c r="C74">
-        <v>0.82558136999999998</v>
+        <v>3.9742267</v>
       </c>
     </row>
     <row r="75" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A75">
-        <v>5.5914636</v>
+        <v>36.423912000000001</v>
       </c>
       <c r="B75">
-        <v>11.737804000000001</v>
+        <v>24.532608</v>
       </c>
       <c r="C75">
-        <v>9.8963412999999996</v>
+        <v>37.496375999999998</v>
       </c>
     </row>
     <row r="76" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A76">
-        <v>11.818345000000001</v>
+        <v>36.963332999999999</v>
       </c>
       <c r="B76">
-        <v>10.829136999999999</v>
+        <v>11.046666999999999</v>
       </c>
       <c r="C76">
-        <v>3.2607913000000002</v>
+        <v>8.3999995999999992</v>
       </c>
     </row>
     <row r="77" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A77">
-        <v>11.956250000000001</v>
+        <v>23.620253000000002</v>
       </c>
       <c r="B77">
-        <v>4.03125</v>
+        <v>2.7943039000000001</v>
       </c>
       <c r="C77">
-        <v>8.7749995999999992</v>
+        <v>3.0632910999999998</v>
       </c>
     </row>
     <row r="78" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A78">
-        <v>5.4785713999999999</v>
+        <v>35.449916999999999</v>
       </c>
       <c r="B78">
-        <v>1.9738095</v>
+        <v>12.568447000000001</v>
       </c>
       <c r="C78">
-        <v>7.9261904000000003</v>
+        <v>16.668613000000001</v>
       </c>
     </row>
     <row r="79" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A79">
-        <v>8.9166670000000003</v>
+        <v>5.2504764000000002</v>
       </c>
       <c r="B79">
-        <v>9.4166670000000003</v>
+        <v>20.896191000000002</v>
       </c>
       <c r="C79">
-        <v>0.45833333999999998</v>
+        <v>36.621906000000003</v>
       </c>
     </row>
     <row r="80" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A80">
-        <v>9.5456991000000002</v>
+        <v>32.347133999999997</v>
       </c>
       <c r="B80">
-        <v>3.6559140999999999</v>
+        <v>4.1815286</v>
       </c>
       <c r="C80">
-        <v>8.9758061999999992</v>
+        <v>2.4745224000000001</v>
       </c>
     </row>
     <row r="81" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A81">
-        <v>0.85185188000000001</v>
+        <v>26.142665999999998</v>
       </c>
       <c r="B81">
-        <v>9.4629630999999996</v>
+        <v>29.124001</v>
       </c>
       <c r="C81">
-        <v>9.8148146000000001</v>
+        <v>38.251998999999998</v>
       </c>
     </row>
     <row r="82" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A82">
-        <v>11.905340000000001</v>
+        <v>14.171480000000001</v>
       </c>
       <c r="B82">
-        <v>1.8325243</v>
+        <v>30.851624999999999</v>
       </c>
       <c r="C82">
-        <v>8.3033981000000008</v>
+        <v>14.265343</v>
       </c>
     </row>
     <row r="83" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A83">
-        <v>12.026596</v>
+        <v>14.060387</v>
       </c>
       <c r="B83">
-        <v>12.063829</v>
+        <v>2.8574879000000002</v>
       </c>
       <c r="C83">
-        <v>13.244680000000001</v>
+        <v>24.693237</v>
       </c>
     </row>
     <row r="84" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A84">
-        <v>12.757936000000001</v>
+        <v>11.353062</v>
       </c>
       <c r="B84">
-        <v>12.988095</v>
+        <v>16.446939</v>
       </c>
       <c r="C84">
-        <v>3.8293650000000001</v>
+        <v>2.9530612999999999</v>
       </c>
     </row>
     <row r="85" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A85">
-        <v>13.576923000000001</v>
+        <v>37.562671999999999</v>
       </c>
       <c r="B85">
-        <v>3.2115385999999999</v>
+        <v>4.4400544000000002</v>
       </c>
       <c r="C85">
-        <v>3.7884614000000001</v>
+        <v>21.020434999999999</v>
       </c>
     </row>
     <row r="86" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A86">
-        <v>0.65972220999999998</v>
+        <v>18.591132999999999</v>
       </c>
       <c r="B86">
-        <v>3.7430555999999999</v>
+        <v>19.194582</v>
       </c>
       <c r="C86">
-        <v>6.7847223000000003</v>
+        <v>25.014778</v>
       </c>
     </row>
     <row r="87" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A87">
-        <v>6.7094592999999998</v>
+        <v>15.277089999999999</v>
       </c>
       <c r="B87">
-        <v>6.6486486999999999</v>
+        <v>37.304955</v>
       </c>
       <c r="C87">
-        <v>9.8378382000000002</v>
+        <v>22.48452</v>
       </c>
     </row>
     <row r="88" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A88">
-        <v>9.046875</v>
+        <v>24.6203</v>
       </c>
       <c r="B88">
-        <v>13.058593999999999</v>
+        <v>13.041353000000001</v>
       </c>
       <c r="C88">
-        <v>2.1289063000000001</v>
+        <v>26.136590999999999</v>
       </c>
     </row>
     <row r="89" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A89">
-        <v>6.4814816000000004</v>
+        <v>17.272151999999998</v>
       </c>
       <c r="B89">
-        <v>7.6296296000000003</v>
+        <v>27.839663000000002</v>
       </c>
       <c r="C89">
-        <v>13.361110999999999</v>
+        <v>23.468354999999999</v>
       </c>
     </row>
     <row r="90" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A90">
-        <v>3.6822032999999998</v>
+        <v>31.917581999999999</v>
       </c>
       <c r="B90">
-        <v>8.6483048999999994</v>
+        <v>7.6428570999999996</v>
       </c>
       <c r="C90">
-        <v>6.9872880000000004</v>
+        <v>26.945055</v>
       </c>
     </row>
     <row r="91" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A91">
-        <v>3.8736557999999999</v>
+        <v>24.184653999999998</v>
       </c>
       <c r="B91">
-        <v>3.9381721000000001</v>
+        <v>25.452781999999999</v>
       </c>
       <c r="C91">
-        <v>5.7553763</v>
+        <v>26.387014000000001</v>
       </c>
     </row>
     <row r="92" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A92">
-        <v>9.7672415000000008</v>
+        <v>31.002203000000002</v>
       </c>
       <c r="B92">
-        <v>12.818966</v>
+        <v>19.026432</v>
       </c>
       <c r="C92">
-        <v>3.2844826999999999</v>
+        <v>37.522025999999997</v>
       </c>
     </row>
     <row r="93" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A93">
-        <v>10.75</v>
+        <v>33.809443999999999</v>
       </c>
       <c r="B93">
-        <v>2.425926</v>
+        <v>32.695438000000003</v>
       </c>
       <c r="C93">
-        <v>1.0185185999999999</v>
+        <v>27.447883999999998</v>
       </c>
     </row>
     <row r="94" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A94">
-        <v>1.7826797999999999</v>
+        <v>37.802883000000001</v>
       </c>
       <c r="B94">
-        <v>1.2892157</v>
+        <v>3.8798077000000002</v>
       </c>
       <c r="C94">
-        <v>1.0310458</v>
+        <v>6.625</v>
       </c>
     </row>
     <row r="95" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A95">
-        <v>6.7907409999999997</v>
+        <v>36.322932999999999</v>
       </c>
       <c r="B95">
-        <v>3.6537036999999999</v>
+        <v>35.473877000000002</v>
       </c>
       <c r="C95">
-        <v>10.546296</v>
+        <v>14.044267</v>
       </c>
     </row>
     <row r="96" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A96">
-        <v>2.4027777000000001</v>
+        <v>34.242736999999998</v>
       </c>
       <c r="B96">
-        <v>9.7361106999999993</v>
+        <v>22.188797000000001</v>
       </c>
       <c r="C96">
-        <v>1.8055555999999999</v>
+        <v>27.022821</v>
       </c>
     </row>
     <row r="97" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A97">
-        <v>10.633333</v>
+        <v>26.211790000000001</v>
       </c>
       <c r="B97">
-        <v>10.75</v>
+        <v>10.002183</v>
       </c>
       <c r="C97">
-        <v>5.6833334000000004</v>
+        <v>2.0851529000000002</v>
       </c>
     </row>
     <row r="98" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A98">
-        <v>7.9110575000000001</v>
+        <v>3.4900498</v>
       </c>
       <c r="B98">
-        <v>4.8485575000000001</v>
+        <v>37.412936999999999</v>
       </c>
       <c r="C98">
-        <v>6.9543271000000004</v>
+        <v>5.0099501999999996</v>
       </c>
     </row>
     <row r="99" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A99">
-        <v>3.8986486999999999</v>
+        <v>13.327089000000001</v>
       </c>
       <c r="B99">
-        <v>4.3716216000000001</v>
+        <v>31.502882</v>
       </c>
       <c r="C99">
-        <v>7.6891889999999998</v>
+        <v>36.972622000000001</v>
       </c>
     </row>
     <row r="100" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A100">
-        <v>2.7205881999999999</v>
+        <v>19.06691</v>
       </c>
       <c r="B100">
-        <v>8.5588236000000002</v>
+        <v>7.6484183999999997</v>
       </c>
       <c r="C100">
-        <v>0.76470590000000005</v>
+        <v>22.336983</v>
       </c>
     </row>
     <row r="101" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A101">
-        <v>6.25</v>
+        <v>23.218309000000001</v>
       </c>
       <c r="B101">
-        <v>9.1666670000000003</v>
+        <v>11</v>
       </c>
       <c r="C101">
-        <v>2.8134920999999999</v>
+        <v>5.8661970999999999</v>
       </c>
     </row>
     <row r="102" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A102">
-        <v>1.0718391</v>
+        <v>2.5748663000000001</v>
       </c>
       <c r="B102">
-        <v>5.1120691000000003</v>
+        <v>21.762032000000001</v>
       </c>
       <c r="C102">
-        <v>10.227012</v>
+        <v>2.4839573000000001</v>
       </c>
     </row>
     <row r="103" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A103">
-        <v>11.117925</v>
+        <v>2.640625</v>
       </c>
       <c r="B103">
-        <v>5.8066038999999998</v>
+        <v>36.416668000000001</v>
       </c>
       <c r="C103">
-        <v>1.2877358000000001</v>
+        <v>29.588540999999999</v>
       </c>
     </row>
     <row r="104" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A104">
-        <v>5.9383115999999996</v>
+        <v>7.4210525000000001</v>
       </c>
       <c r="B104">
-        <v>0.92532468000000001</v>
+        <v>33.109650000000002</v>
       </c>
       <c r="C104">
-        <v>12.730518999999999</v>
+        <v>21.592106000000001</v>
       </c>
     </row>
     <row r="105" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A105">
-        <v>2.8344157000000001</v>
+        <v>15.802752</v>
       </c>
       <c r="B105">
-        <v>2.9058442000000002</v>
+        <v>38.490825999999998</v>
       </c>
       <c r="C105">
-        <v>12.009740000000001</v>
+        <v>2.9128438999999999</v>
       </c>
     </row>
     <row r="106" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A106">
-        <v>0.67372882000000001</v>
+        <v>29.494817999999999</v>
       </c>
       <c r="B106">
-        <v>10.377119</v>
+        <v>2.2409327000000001</v>
       </c>
       <c r="C106">
-        <v>3.5720339000000001</v>
+        <v>34.152850999999998</v>
       </c>
     </row>
     <row r="107" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A107">
-        <v>3.8892045</v>
+        <v>17.131124</v>
       </c>
       <c r="B107">
-        <v>11.883523</v>
+        <v>2.5605186999999998</v>
       </c>
       <c r="C107">
-        <v>8.0397730000000003</v>
+        <v>37.056193999999998</v>
       </c>
     </row>
     <row r="108" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A108">
-        <v>11.632353</v>
+        <v>12.919192000000001</v>
       </c>
       <c r="B108">
-        <v>0.65196078999999996</v>
+        <v>22.611111000000001</v>
       </c>
       <c r="C108">
-        <v>6.0931373000000004</v>
+        <v>38.181820000000002</v>
       </c>
     </row>
     <row r="109" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A109">
-        <v>11.850529</v>
+        <v>35.537692999999997</v>
       </c>
       <c r="B109">
-        <v>3.7949736000000001</v>
+        <v>3.0144123999999999</v>
       </c>
       <c r="C109">
-        <v>5.8505292000000004</v>
+        <v>29.619734000000001</v>
       </c>
     </row>
     <row r="110" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A110">
-        <v>1.2153678999999999</v>
+        <v>28.999006000000001</v>
       </c>
       <c r="B110">
-        <v>1.6937230000000001</v>
+        <v>28.666998</v>
       </c>
       <c r="C110">
-        <v>3.7456710000000002</v>
+        <v>33.746521000000001</v>
       </c>
     </row>
     <row r="111" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A111">
-        <v>9.0335053999999992</v>
+        <v>37.806725</v>
       </c>
       <c r="B111">
-        <v>12.46134</v>
+        <v>18.592438000000001</v>
       </c>
       <c r="C111">
-        <v>12.489691000000001</v>
+        <v>31.481092</v>
       </c>
     </row>
     <row r="112" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A112">
-        <v>4.0755815999999996</v>
+        <v>1.9591837000000001</v>
       </c>
       <c r="B112">
-        <v>0.76162790999999996</v>
+        <v>10.959184</v>
       </c>
       <c r="C112">
-        <v>10.843023000000001</v>
+        <v>30.448979999999999</v>
       </c>
     </row>
     <row r="113" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A113">
-        <v>3.6753730999999998</v>
+        <v>38.186047000000002</v>
       </c>
       <c r="B113">
-        <v>1.9962686000000001</v>
+        <v>13.011628</v>
       </c>
       <c r="C113">
-        <v>3.4813432999999998</v>
+        <v>22.647286999999999</v>
       </c>
     </row>
     <row r="114" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A114">
-        <v>0.77205884000000002</v>
+        <v>37.241379000000002</v>
       </c>
       <c r="B114">
-        <v>2.3602941</v>
+        <v>38.474136000000001</v>
       </c>
       <c r="C114">
-        <v>10.713234999999999</v>
+        <v>36.689655000000002</v>
       </c>
     </row>
     <row r="115" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A115">
-        <v>12.943548</v>
+        <v>2.5543933000000001</v>
       </c>
       <c r="B115">
-        <v>10.787635</v>
+        <v>29.650627</v>
       </c>
       <c r="C115">
-        <v>7.0887098000000002</v>
+        <v>27.303346999999999</v>
       </c>
     </row>
     <row r="116" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A116">
-        <v>11.273255000000001</v>
+        <v>29.690617</v>
       </c>
       <c r="B116">
-        <v>2.0988370999999999</v>
+        <v>23.802053000000001</v>
       </c>
       <c r="C116">
-        <v>12.273255000000001</v>
+        <v>22.101172999999999</v>
       </c>
     </row>
     <row r="117" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A117">
-        <v>1.6650944000000001</v>
+        <v>7.1801348000000003</v>
       </c>
       <c r="B117">
-        <v>2.8915095000000002</v>
+        <v>37.153198000000003</v>
       </c>
       <c r="C117">
-        <v>8.7264146999999994</v>
+        <v>13.355219</v>
       </c>
     </row>
     <row r="118" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A118">
-        <v>1.8846153999999999</v>
+        <v>8.0340232999999994</v>
       </c>
       <c r="B118">
-        <v>8.6730765999999999</v>
+        <v>13.744082000000001</v>
       </c>
       <c r="C118">
-        <v>10.673076999999999</v>
+        <v>11.619823</v>
       </c>
     </row>
     <row r="119" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A119">
-        <v>3.6681819</v>
+        <v>27.358778000000001</v>
       </c>
       <c r="B119">
-        <v>6.0954547000000003</v>
+        <v>6.7442745999999998</v>
       </c>
       <c r="C119">
-        <v>13.340909</v>
+        <v>38.461834000000003</v>
       </c>
     </row>
     <row r="120" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A120">
-        <v>1.3401639000000001</v>
+        <v>9.6931820000000002</v>
       </c>
       <c r="B120">
-        <v>0.84836065999999999</v>
+        <v>19.261364</v>
       </c>
       <c r="C120">
-        <v>11.610656000000001</v>
+        <v>33.147728000000001</v>
       </c>
     </row>
     <row r="121" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A121">
-        <v>13.607142</v>
+        <v>29.310759999999998</v>
       </c>
       <c r="B121">
-        <v>8.8214283000000009</v>
+        <v>20.021336000000002</v>
       </c>
       <c r="C121">
-        <v>3.5357143999999998</v>
+        <v>31.260667999999999</v>
       </c>
     </row>
     <row r="122" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A122">
-        <v>6.6458335000000002</v>
+        <v>30.031084</v>
       </c>
       <c r="B122">
-        <v>5.9375</v>
+        <v>5.8090586999999996</v>
       </c>
       <c r="C122">
-        <v>12.840278</v>
+        <v>7.8285966</v>
       </c>
     </row>
     <row r="123" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A123">
-        <v>6.1206899000000003</v>
+        <v>18.461303999999998</v>
       </c>
       <c r="B123">
-        <v>1.612069</v>
+        <v>3.212831</v>
       </c>
       <c r="C123">
-        <v>9.9741382999999999</v>
+        <v>16.231161</v>
       </c>
     </row>
     <row r="124" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A124">
-        <v>3.7981482</v>
+        <v>1.9418603999999999</v>
       </c>
       <c r="B124">
-        <v>5.8574076000000002</v>
+        <v>3</v>
       </c>
       <c r="C124">
-        <v>11.603702999999999</v>
+        <v>28.36628</v>
       </c>
     </row>
     <row r="125" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A125">
-        <v>11.106</v>
+        <v>20.131819</v>
       </c>
       <c r="B125">
-        <v>6.4660000999999996</v>
+        <v>2.2772727000000001</v>
       </c>
       <c r="C125">
-        <v>4.8019999999999996</v>
+        <v>26.154544999999999</v>
       </c>
     </row>
     <row r="126" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A126">
-        <v>10.941011</v>
+        <v>21.882670999999998</v>
       </c>
       <c r="B126">
-        <v>3.9634830999999999</v>
+        <v>10.985559</v>
       </c>
       <c r="C126">
-        <v>1.1095505999999999</v>
+        <v>14.223826000000001</v>
       </c>
     </row>
     <row r="127" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A127">
-        <v>13.098485</v>
+        <v>13.389830999999999</v>
       </c>
       <c r="B127">
-        <v>8.8762626999999998</v>
+        <v>38.067794999999997</v>
       </c>
       <c r="C127">
-        <v>4.4772724999999998</v>
+        <v>10.203390000000001</v>
       </c>
     </row>
     <row r="128" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A128">
-        <v>4.0725807999999999</v>
+        <v>10.555908000000001</v>
       </c>
       <c r="B128">
-        <v>3.7419354999999999</v>
+        <v>30.834181000000001</v>
       </c>
       <c r="C128">
-        <v>3.9274193999999998</v>
+        <v>28.976493999999999</v>
       </c>
     </row>
     <row r="129" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A129">
-        <v>8.4598216999999991</v>
+        <v>2.4090910000000001</v>
       </c>
       <c r="B129">
-        <v>9.6741075999999993</v>
+        <v>36.483471000000002</v>
       </c>
       <c r="C129">
-        <v>11.4375</v>
+        <v>23.772728000000001</v>
       </c>
     </row>
     <row r="130" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A130">
-        <v>10.311225</v>
+        <v>23.124243</v>
       </c>
       <c r="B130">
-        <v>0.99489795999999997</v>
+        <v>38.324241999999998</v>
       </c>
       <c r="C130">
-        <v>13.392858</v>
+        <v>3.3606060000000002</v>
       </c>
     </row>
     <row r="131" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A131">
-        <v>1.0373564</v>
+        <v>9.8549042</v>
       </c>
       <c r="B131">
-        <v>5.0890803</v>
+        <v>5.4625883000000002</v>
       </c>
       <c r="C131">
-        <v>4.1293100999999997</v>
+        <v>18.068251</v>
       </c>
     </row>
     <row r="132" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A132">
-        <v>5.9078945999999997</v>
+        <v>4.5141343999999997</v>
       </c>
       <c r="B132">
-        <v>7.2236843000000004</v>
+        <v>37.765017999999998</v>
       </c>
       <c r="C132">
-        <v>6.8728069999999999</v>
+        <v>18.471730999999998</v>
       </c>
     </row>
     <row r="133" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A133">
-        <v>3.0247251999999998</v>
+        <v>32.961421999999999</v>
       </c>
       <c r="B133">
-        <v>10.326923000000001</v>
+        <v>24.891829999999999</v>
       </c>
       <c r="C133">
-        <v>13.14011</v>
+        <v>14.905446</v>
       </c>
     </row>
     <row r="134" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A134">
-        <v>8</v>
+        <v>8.5306748999999993</v>
       </c>
       <c r="B134">
-        <v>0.78571427000000005</v>
+        <v>14.493865</v>
       </c>
       <c r="C134">
-        <v>12.946427999999999</v>
+        <v>21.902863</v>
       </c>
     </row>
     <row r="135" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A135">
-        <v>0.95270270000000001</v>
+        <v>37.272387999999999</v>
       </c>
       <c r="B135">
-        <v>13.128378</v>
+        <v>32.578358000000001</v>
       </c>
       <c r="C135">
-        <v>8.1621617999999998</v>
+        <v>37.190300000000001</v>
       </c>
     </row>
     <row r="136" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A136">
-        <v>4.7628206999999998</v>
+        <v>2.5759257999999998</v>
       </c>
       <c r="B136">
-        <v>1.0961539</v>
+        <v>13.407408</v>
       </c>
       <c r="C136">
-        <v>2.4551281999999999</v>
+        <v>16.203703000000001</v>
       </c>
     </row>
     <row r="137" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A137">
-        <v>13.278302</v>
+        <v>21.369347000000001</v>
       </c>
       <c r="B137">
-        <v>6.6556601999999998</v>
+        <v>15.886934</v>
       </c>
       <c r="C137">
-        <v>5.0801888000000002</v>
+        <v>31.753768999999998</v>
       </c>
     </row>
     <row r="138" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A138">
-        <v>0.91470587000000003</v>
+        <v>32.209999000000003</v>
       </c>
       <c r="B138">
-        <v>10.767647</v>
+        <v>13.808332999999999</v>
       </c>
       <c r="C138">
-        <v>8.7147055000000009</v>
+        <v>26.030000999999999</v>
       </c>
     </row>
     <row r="139" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A139">
-        <v>7.03125</v>
+        <v>27.434334</v>
       </c>
       <c r="B139">
-        <v>6.0625</v>
+        <v>15.436210000000001</v>
       </c>
       <c r="C139">
-        <v>6.65625</v>
+        <v>19.655722000000001</v>
       </c>
     </row>
     <row r="140" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A140">
-        <v>3.7111649999999998</v>
+        <v>3.3856305999999998</v>
       </c>
       <c r="B140">
-        <v>10.036407000000001</v>
+        <v>33.060116000000001</v>
       </c>
       <c r="C140">
-        <v>10.929611</v>
+        <v>38.180351000000002</v>
       </c>
     </row>
     <row r="141" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A141">
-        <v>9.0153847000000003</v>
+        <v>20.540419</v>
       </c>
       <c r="B141">
-        <v>13.373077</v>
+        <v>34.661678000000002</v>
       </c>
       <c r="C141">
-        <v>8.9576920999999992</v>
+        <v>31.980539</v>
       </c>
     </row>
     <row r="142" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A142">
-        <v>5.8939395000000001</v>
+        <v>24.417562</v>
       </c>
       <c r="B142">
-        <v>5.5530305000000002</v>
+        <v>17.593188999999999</v>
       </c>
       <c r="C142">
-        <v>8.8257580000000004</v>
+        <v>2.7150538000000002</v>
       </c>
     </row>
     <row r="143" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A143">
-        <v>1.8686441</v>
+        <v>13.509983</v>
       </c>
       <c r="B143">
-        <v>6.0127119999999996</v>
+        <v>23.178868999999999</v>
       </c>
       <c r="C143">
-        <v>2.4110168999999999</v>
+        <v>29.990849000000001</v>
       </c>
     </row>
     <row r="144" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A144">
-        <v>12.162463000000001</v>
+        <v>3.2574369999999999</v>
       </c>
       <c r="B144">
-        <v>12.198071000000001</v>
+        <v>13.069794</v>
       </c>
       <c r="C144">
-        <v>10.031898999999999</v>
+        <v>36.721969999999999</v>
       </c>
     </row>
     <row r="145" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A145">
-        <v>6.4739585000000002</v>
+        <v>3.3561451</v>
       </c>
       <c r="B145">
-        <v>3.5729166999999999</v>
+        <v>29.536311999999999</v>
       </c>
       <c r="C145">
-        <v>3.7708333000000001</v>
+        <v>5.8617319999999999</v>
       </c>
     </row>
     <row r="146" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A146">
-        <v>5.9817071000000004</v>
+        <v>3.7249173999999998</v>
       </c>
       <c r="B146">
-        <v>10.554878</v>
+        <v>25.869350000000001</v>
       </c>
       <c r="C146">
-        <v>1.054878</v>
+        <v>18.125136999999999</v>
       </c>
     </row>
     <row r="147" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A147">
-        <v>1.7258065</v>
+        <v>8.7307691999999992</v>
       </c>
       <c r="B147">
-        <v>4.3306450999999999</v>
+        <v>37.991450999999998</v>
       </c>
       <c r="C147">
-        <v>13.419354</v>
+        <v>27.324787000000001</v>
       </c>
     </row>
     <row r="148" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A148">
-        <v>0.47499998999999998</v>
+        <v>31.399145000000001</v>
       </c>
       <c r="B148">
-        <v>10.425000000000001</v>
+        <v>3.6743591000000002</v>
       </c>
       <c r="C148">
-        <v>7.1999997999999996</v>
+        <v>17.705127999999998</v>
       </c>
     </row>
     <row r="149" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A149">
-        <v>7.7134147000000004</v>
+        <v>24.074684000000001</v>
       </c>
       <c r="B149">
-        <v>9.9817076</v>
+        <v>3.1075949999999999</v>
       </c>
       <c r="C149">
-        <v>13.408537000000001</v>
+        <v>10.279747</v>
       </c>
     </row>
     <row r="150" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A150">
-        <v>13.003333</v>
+        <v>25.681208000000002</v>
       </c>
       <c r="B150">
-        <v>6.8366666</v>
+        <v>6.3076062000000004</v>
       </c>
       <c r="C150">
-        <v>12.683332999999999</v>
+        <v>17.895973000000001</v>
       </c>
     </row>
     <row r="151" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A151">
-        <v>9.836957</v>
+        <v>27.056336999999999</v>
       </c>
       <c r="B151">
-        <v>4.9782609999999998</v>
+        <v>32.17371</v>
       </c>
       <c r="C151">
-        <v>3.8369564999999999</v>
+        <v>10.267606000000001</v>
       </c>
     </row>
     <row r="152" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A152">
-        <v>1.0036764</v>
+        <v>10.469267</v>
       </c>
       <c r="B152">
-        <v>6.7352942999999996</v>
+        <v>37.445625</v>
       </c>
       <c r="C152">
-        <v>6.0551472000000004</v>
+        <v>35.800235999999998</v>
       </c>
     </row>
     <row r="153" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A153">
-        <v>5.9115386000000001</v>
+        <v>38.285713000000001</v>
       </c>
       <c r="B153">
-        <v>2.8269231000000001</v>
+        <v>2.2232143999999998</v>
       </c>
       <c r="C153">
-        <v>12.657692000000001</v>
+        <v>36.794643000000001</v>
       </c>
     </row>
     <row r="154" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A154">
-        <v>10.511628</v>
+        <v>16.072051999999999</v>
       </c>
       <c r="B154">
-        <v>12.040698000000001</v>
+        <v>2.687773</v>
       </c>
       <c r="C154">
-        <v>6.9069767000000004</v>
+        <v>9.5917034000000001</v>
       </c>
     </row>
     <row r="155" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A155">
-        <v>12.764851999999999</v>
+        <v>37.055557</v>
       </c>
       <c r="B155">
-        <v>3.0420791999999999</v>
+        <v>19.113636</v>
       </c>
       <c r="C155">
-        <v>11.155941</v>
+        <v>9.7828283000000003</v>
       </c>
     </row>
     <row r="156" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A156">
-        <v>1.2424242000000001</v>
+        <v>34.110767000000003</v>
       </c>
       <c r="B156">
-        <v>11.511364</v>
+        <v>29.444790000000001</v>
       </c>
       <c r="C156">
-        <v>6.3409089999999999</v>
+        <v>5.0051760999999999</v>
       </c>
     </row>
     <row r="157" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A157">
-        <v>12.835227</v>
+        <v>2.2522935999999998</v>
       </c>
       <c r="B157">
-        <v>10.454545</v>
+        <v>25.981650999999999</v>
       </c>
       <c r="C157">
-        <v>5.2272724999999998</v>
+        <v>33.724769999999999</v>
       </c>
     </row>
     <row r="158" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A158">
-        <v>8.6997490000000006</v>
+        <v>38.227271999999999</v>
       </c>
       <c r="B158">
-        <v>6.8655777000000002</v>
+        <v>36.386364</v>
       </c>
       <c r="C158">
-        <v>10.089195999999999</v>
+        <v>32.079543999999999</v>
       </c>
     </row>
     <row r="159" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A159">
-        <v>6.5878376999999997</v>
+        <v>28.190037</v>
       </c>
       <c r="B159">
-        <v>12.763514000000001</v>
+        <v>34.293357999999998</v>
       </c>
       <c r="C159">
-        <v>8.8175678000000008</v>
+        <v>26.289667000000001</v>
       </c>
     </row>
     <row r="160" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A160">
-        <v>8.9026718000000002</v>
+        <v>19.916847000000001</v>
       </c>
       <c r="B160">
-        <v>12.875954999999999</v>
+        <v>16.813175000000001</v>
       </c>
       <c r="C160">
-        <v>5.5667939000000004</v>
+        <v>9.9924402000000008</v>
       </c>
     </row>
     <row r="161" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A161">
-        <v>5.8881763999999999</v>
+        <v>15.604022000000001</v>
       </c>
       <c r="B161">
-        <v>8.9408835999999994</v>
+        <v>16.567961</v>
       </c>
       <c r="C161">
-        <v>9.5548429000000006</v>
+        <v>17.161581000000002</v>
       </c>
     </row>
     <row r="162" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A162">
-        <v>5.3703703999999997</v>
+        <v>6.6893940000000001</v>
       </c>
       <c r="B162">
-        <v>13.361110999999999</v>
+        <v>9.0707073000000005</v>
       </c>
       <c r="C162">
-        <v>9.6296301</v>
+        <v>30.512626999999998</v>
       </c>
     </row>
     <row r="163" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A163">
-        <v>6.0192307999999999</v>
+        <v>27.737431000000001</v>
       </c>
       <c r="B163">
-        <v>13.538462000000001</v>
+        <v>23.477654000000001</v>
       </c>
       <c r="C163">
-        <v>13.403846</v>
+        <v>5.6983242000000001</v>
       </c>
     </row>
     <row r="164" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A164">
-        <v>3.8289472999999998</v>
+        <v>3.4527364</v>
       </c>
       <c r="B164">
-        <v>3.5438597000000001</v>
+        <v>8.1641788000000002</v>
       </c>
       <c r="C164">
-        <v>1.0175438999999999</v>
+        <v>2.8532337999999999</v>
       </c>
     </row>
     <row r="165" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A165">
-        <v>3.5094935999999999</v>
+        <v>10.744047</v>
       </c>
       <c r="B165">
-        <v>6.6803799000000001</v>
+        <v>34.125</v>
       </c>
       <c r="C165">
-        <v>5.8322782999999996</v>
-      </c>
-    </row>
-    <row r="166" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A166">
-        <v>0.75724638</v>
-      </c>
-      <c r="B166">
-        <v>12.438406000000001</v>
-      </c>
-      <c r="C166">
-        <v>0.89492755999999996</v>
-      </c>
-    </row>
-    <row r="167" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A167">
-        <v>4.6458335000000002</v>
-      </c>
-      <c r="B167">
-        <v>7.6666664999999998</v>
-      </c>
-      <c r="C167">
-        <v>2.6666666999999999</v>
-      </c>
-    </row>
-    <row r="168" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A168">
-        <v>11.75</v>
-      </c>
-      <c r="B168">
-        <v>5.7916664999999998</v>
-      </c>
-      <c r="C168">
-        <v>11.638889000000001</v>
-      </c>
-    </row>
-    <row r="169" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A169">
-        <v>9.8788661999999992</v>
-      </c>
-      <c r="B169">
-        <v>9.9149484999999995</v>
-      </c>
-      <c r="C169">
-        <v>1.1520618</v>
-      </c>
-    </row>
-    <row r="170" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A170">
-        <v>1.0247253000000001</v>
-      </c>
-      <c r="B170">
-        <v>12.898351999999999</v>
-      </c>
-      <c r="C170">
-        <v>4.5302195999999997</v>
-      </c>
-    </row>
-    <row r="171" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A171">
-        <v>2.3474026000000001</v>
-      </c>
-      <c r="B171">
-        <v>12.925324</v>
-      </c>
-      <c r="C171">
-        <v>10.555194999999999</v>
-      </c>
-    </row>
-    <row r="172" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A172">
-        <v>3.7246377000000002</v>
-      </c>
-      <c r="B172">
-        <v>10.115942</v>
-      </c>
-      <c r="C172">
-        <v>5.6739129999999998</v>
-      </c>
-    </row>
-    <row r="173" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A173">
-        <v>4.9435482000000004</v>
-      </c>
-      <c r="B173">
-        <v>9.0564517999999996</v>
-      </c>
-      <c r="C173">
-        <v>13.620968</v>
-      </c>
-    </row>
-    <row r="174" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A174">
-        <v>11.735075</v>
-      </c>
-      <c r="B174">
-        <v>9.8843279000000006</v>
-      </c>
-      <c r="C174">
-        <v>13.108209</v>
-      </c>
-    </row>
-    <row r="175" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A175">
-        <v>11.044737</v>
-      </c>
-      <c r="B175">
-        <v>6.9499997999999996</v>
-      </c>
-      <c r="C175">
-        <v>10.086843</v>
-      </c>
-    </row>
-    <row r="176" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A176">
-        <v>12.809524</v>
-      </c>
-      <c r="B176">
-        <v>12.452381000000001</v>
-      </c>
-      <c r="C176">
-        <v>6.6904763999999997</v>
-      </c>
-    </row>
-    <row r="177" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A177">
-        <v>2.4486300999999999</v>
-      </c>
-      <c r="B177">
-        <v>0.70890408999999999</v>
-      </c>
-      <c r="C177">
-        <v>9.6472607000000004</v>
-      </c>
-    </row>
-    <row r="178" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A178">
-        <v>4.962707</v>
-      </c>
-      <c r="B178">
-        <v>11.935082</v>
-      </c>
-      <c r="C178">
-        <v>12.714088</v>
-      </c>
-    </row>
-    <row r="179" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A179">
-        <v>8.8255204999999997</v>
-      </c>
-      <c r="B179">
-        <v>8.3619795000000003</v>
-      </c>
-      <c r="C179">
-        <v>5.8489585000000002</v>
-      </c>
-    </row>
-    <row r="180" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A180">
-        <v>2.7107329</v>
-      </c>
-      <c r="B180">
-        <v>9.5510473000000005</v>
-      </c>
-      <c r="C180">
-        <v>8.6243458000000004</v>
-      </c>
-    </row>
-    <row r="181" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A181">
-        <v>6.8706899000000003</v>
-      </c>
-      <c r="B181">
-        <v>1.1580459999999999</v>
-      </c>
-      <c r="C181">
-        <v>3.8477011000000001</v>
-      </c>
-    </row>
-    <row r="182" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A182">
-        <v>8.8728064999999994</v>
-      </c>
-      <c r="B182">
-        <v>2.8201754000000001</v>
-      </c>
-      <c r="C182">
-        <v>13.416667</v>
-      </c>
-    </row>
-    <row r="183" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A183">
-        <v>9.7870369000000004</v>
-      </c>
-      <c r="B183">
-        <v>10.175926</v>
-      </c>
-      <c r="C183">
-        <v>13.268518</v>
-      </c>
-    </row>
-    <row r="184" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A184">
-        <v>13.08</v>
-      </c>
-      <c r="B184">
-        <v>5.085</v>
-      </c>
-      <c r="C184">
-        <v>1.0049999999999999</v>
-      </c>
-    </row>
-    <row r="185" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A185">
-        <v>7.0431032</v>
-      </c>
-      <c r="B185">
-        <v>0.75</v>
-      </c>
-      <c r="C185">
-        <v>9.0603446999999999</v>
-      </c>
-    </row>
-    <row r="186" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A186">
-        <v>6.6029410000000004</v>
-      </c>
-      <c r="B186">
-        <v>1.8205882</v>
-      </c>
-      <c r="C186">
-        <v>1.0911765</v>
-      </c>
-    </row>
-    <row r="187" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A187">
-        <v>8.9166670000000003</v>
-      </c>
-      <c r="B187">
-        <v>7.2333331000000003</v>
-      </c>
-      <c r="C187">
-        <v>8.6166668000000008</v>
-      </c>
-    </row>
-    <row r="188" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A188">
-        <v>1.0323529</v>
-      </c>
-      <c r="B188">
-        <v>7.1852942000000004</v>
-      </c>
-      <c r="C188">
-        <v>8.5617646999999995</v>
-      </c>
-    </row>
-    <row r="189" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A189">
-        <v>4.9939022</v>
-      </c>
-      <c r="B189">
-        <v>13.432926999999999</v>
-      </c>
-      <c r="C189">
-        <v>10.896341</v>
-      </c>
-    </row>
-    <row r="190" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A190">
-        <v>9.5915488999999994</v>
-      </c>
-      <c r="B190">
-        <v>0.97183096000000002</v>
-      </c>
-      <c r="C190">
-        <v>10.573943999999999</v>
-      </c>
-    </row>
-    <row r="191" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A191">
-        <v>10.476191</v>
-      </c>
-      <c r="B191">
-        <v>9.9226188999999998</v>
-      </c>
-      <c r="C191">
-        <v>11.458333</v>
-      </c>
-    </row>
-    <row r="192" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A192">
-        <v>4.9055556999999999</v>
-      </c>
-      <c r="B192">
-        <v>10.638889000000001</v>
-      </c>
-      <c r="C192">
-        <v>1.0277778</v>
-      </c>
-    </row>
-    <row r="193" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A193">
-        <v>9.6512870999999993</v>
-      </c>
-      <c r="B193">
-        <v>1.5075107999999999</v>
-      </c>
-      <c r="C193">
-        <v>5.9581546999999997</v>
-      </c>
-    </row>
-    <row r="194" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A194">
-        <v>1.0733334000000001</v>
-      </c>
-      <c r="B194">
-        <v>10.8</v>
-      </c>
-      <c r="C194">
-        <v>12.046666999999999</v>
-      </c>
-    </row>
-    <row r="195" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A195">
-        <v>5.5701217999999999</v>
-      </c>
-      <c r="B195">
-        <v>5.5914636</v>
-      </c>
-      <c r="C195">
-        <v>1.7134147</v>
-      </c>
-    </row>
-    <row r="196" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A196">
-        <v>7.7919846000000001</v>
-      </c>
-      <c r="B196">
-        <v>11.811069</v>
-      </c>
-      <c r="C196">
-        <v>10.818702999999999</v>
-      </c>
-    </row>
-    <row r="197" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A197">
-        <v>3.1333334000000002</v>
-      </c>
-      <c r="B197">
-        <v>1</v>
-      </c>
-      <c r="C197">
-        <v>7.6999997999999996</v>
-      </c>
-    </row>
-    <row r="198" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A198">
-        <v>13.284722</v>
-      </c>
-      <c r="B198">
-        <v>2.7430555999999999</v>
-      </c>
-      <c r="C198">
-        <v>1.6458333999999999</v>
-      </c>
-    </row>
-    <row r="199" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A199">
-        <v>4.7408257000000003</v>
-      </c>
-      <c r="B199">
-        <v>1.2362385</v>
-      </c>
-      <c r="C199">
-        <v>1.0848624</v>
-      </c>
-    </row>
-    <row r="200" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A200">
-        <v>12.655263</v>
-      </c>
-      <c r="B200">
-        <v>6.6500000999999997</v>
-      </c>
-      <c r="C200">
-        <v>7.8394737000000001</v>
-      </c>
-    </row>
-    <row r="201" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A201">
-        <v>8.7102269999999997</v>
-      </c>
-      <c r="B201">
-        <v>10.681818</v>
-      </c>
-      <c r="C201">
-        <v>3.5397726999999999</v>
-      </c>
-    </row>
-    <row r="202" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A202">
-        <v>12.031817999999999</v>
-      </c>
-      <c r="B202">
-        <v>8.7318181999999993</v>
-      </c>
-      <c r="C202">
-        <v>7.7636365999999999</v>
-      </c>
-    </row>
-    <row r="203" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A203">
-        <v>6.5752034000000004</v>
-      </c>
-      <c r="B203">
-        <v>6.5752034000000004</v>
-      </c>
-      <c r="C203">
-        <v>4.1808943999999997</v>
-      </c>
-    </row>
-    <row r="204" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A204">
-        <v>13.266482999999999</v>
-      </c>
-      <c r="B204">
-        <v>10.211537999999999</v>
-      </c>
-      <c r="C204">
-        <v>1.1785715000000001</v>
-      </c>
-    </row>
-    <row r="205" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A205">
-        <v>4.6285714999999996</v>
-      </c>
-      <c r="B205">
-        <v>0.95714283</v>
-      </c>
-      <c r="C205">
-        <v>4.1357141000000004</v>
-      </c>
-    </row>
-    <row r="206" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A206">
-        <v>11.118421</v>
-      </c>
-      <c r="B206">
-        <v>10.776316</v>
-      </c>
-      <c r="C206">
-        <v>7.3552631999999996</v>
-      </c>
-    </row>
-    <row r="207" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A207">
-        <v>8.75</v>
-      </c>
-      <c r="B207">
-        <v>1.4861112000000001</v>
-      </c>
-      <c r="C207">
-        <v>8.7152776999999997</v>
-      </c>
-    </row>
-    <row r="208" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A208">
-        <v>8.8404760000000007</v>
-      </c>
-      <c r="B208">
-        <v>7.6452378999999997</v>
-      </c>
-      <c r="C208">
-        <v>13.078571</v>
-      </c>
-    </row>
-    <row r="209" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A209">
-        <v>5.5833335000000002</v>
-      </c>
-      <c r="B209">
-        <v>5.3277779000000001</v>
-      </c>
-      <c r="C209">
-        <v>4.9166664999999998</v>
-      </c>
-    </row>
-    <row r="210" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A210">
-        <v>10.347015000000001</v>
-      </c>
-      <c r="B210">
-        <v>3.2798506999999999</v>
-      </c>
-      <c r="C210">
-        <v>3.2276120000000001</v>
-      </c>
-    </row>
-    <row r="211" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A211">
-        <v>3.6921053000000001</v>
-      </c>
-      <c r="B211">
-        <v>12.184210999999999</v>
-      </c>
-      <c r="C211">
-        <v>1.4394735999999999</v>
-      </c>
-    </row>
-    <row r="212" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A212">
-        <v>13.5625</v>
-      </c>
-      <c r="B212">
-        <v>5.34375</v>
-      </c>
-      <c r="C212">
-        <v>7.40625</v>
-      </c>
-    </row>
-    <row r="213" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A213">
-        <v>7.7362637999999997</v>
-      </c>
-      <c r="B213">
-        <v>7.8434067000000001</v>
-      </c>
-      <c r="C213">
-        <v>1.7142857</v>
-      </c>
-    </row>
-    <row r="214" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A214">
-        <v>12.841837</v>
-      </c>
-      <c r="B214">
-        <v>7.6071429000000004</v>
-      </c>
-      <c r="C214">
-        <v>0.95408165</v>
-      </c>
-    </row>
-    <row r="215" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A215">
-        <v>0.73333334999999999</v>
-      </c>
-      <c r="B215">
-        <v>12.983333999999999</v>
-      </c>
-      <c r="C215">
-        <v>10.7</v>
-      </c>
-    </row>
-    <row r="216" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A216">
-        <v>0.98611110000000002</v>
-      </c>
-      <c r="B216">
-        <v>13.361110999999999</v>
-      </c>
-      <c r="C216">
-        <v>2.8333333000000001</v>
-      </c>
-    </row>
-    <row r="217" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A217">
-        <v>8.2857140999999999</v>
-      </c>
-      <c r="B217">
-        <v>4.6875</v>
-      </c>
-      <c r="C217">
-        <v>13.526786</v>
-      </c>
-    </row>
-    <row r="218" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A218">
-        <v>13.181578999999999</v>
-      </c>
-      <c r="B218">
-        <v>8.8131579999999996</v>
-      </c>
-      <c r="C218">
-        <v>10.013158000000001</v>
-      </c>
-    </row>
-    <row r="219" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A219">
-        <v>13.196281000000001</v>
-      </c>
-      <c r="B219">
-        <v>5.8119835999999996</v>
-      </c>
-      <c r="C219">
-        <v>10.840909</v>
-      </c>
-    </row>
-    <row r="220" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A220">
-        <v>8.336957</v>
-      </c>
-      <c r="B220">
-        <v>1.7355072</v>
-      </c>
-      <c r="C220">
-        <v>0.91666669000000001</v>
-      </c>
-    </row>
-    <row r="221" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A221">
-        <v>0.89705884000000002</v>
-      </c>
-      <c r="B221">
-        <v>3.7058822999999999</v>
-      </c>
-      <c r="C221">
-        <v>11.992647</v>
-      </c>
-    </row>
-    <row r="222" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A222">
-        <v>3.6117021999999999</v>
-      </c>
-      <c r="B222">
-        <v>6.7287235000000001</v>
-      </c>
-      <c r="C222">
-        <v>3.5691489999999999</v>
-      </c>
-    </row>
-    <row r="223" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A223">
-        <v>1.0792683000000001</v>
-      </c>
-      <c r="B223">
-        <v>1.1371951</v>
-      </c>
-      <c r="C223">
-        <v>7.1128049000000004</v>
-      </c>
-    </row>
-    <row r="224" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A224">
-        <v>11.564569000000001</v>
-      </c>
-      <c r="B224">
-        <v>7.8592715000000002</v>
-      </c>
-      <c r="C224">
-        <v>12.922186</v>
-      </c>
-    </row>
-    <row r="225" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A225">
-        <v>12.585526</v>
-      </c>
-      <c r="B225">
-        <v>4.6743421999999999</v>
-      </c>
-      <c r="C225">
-        <v>3.5460527000000002</v>
-      </c>
-    </row>
-    <row r="226" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A226">
-        <v>10.715909</v>
-      </c>
-      <c r="B226">
-        <v>9.8143940000000001</v>
-      </c>
-      <c r="C226">
-        <v>9.1856059999999999</v>
-      </c>
-    </row>
-    <row r="227" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A227">
-        <v>10.717105</v>
-      </c>
-      <c r="B227">
-        <v>5.8684210999999999</v>
-      </c>
-      <c r="C227">
-        <v>7.7763156999999996</v>
-      </c>
-    </row>
-    <row r="228" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A228">
-        <v>7.0833335000000002</v>
-      </c>
-      <c r="B228">
-        <v>12.592592</v>
-      </c>
-      <c r="C228">
-        <v>7.2962961000000002</v>
-      </c>
-    </row>
-    <row r="229" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A229">
-        <v>3.9076086999999999</v>
-      </c>
-      <c r="B229">
-        <v>1.0652174000000001</v>
-      </c>
-      <c r="C229">
-        <v>12.744565</v>
-      </c>
-    </row>
-    <row r="230" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A230">
-        <v>12.047794</v>
-      </c>
-      <c r="B230">
-        <v>4.4301472000000004</v>
-      </c>
-      <c r="C230">
-        <v>13.202206</v>
-      </c>
-    </row>
-    <row r="231" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A231">
-        <v>9.1184206000000003</v>
-      </c>
-      <c r="B231">
-        <v>11.969298</v>
-      </c>
-      <c r="C231">
-        <v>8.2149123999999993</v>
-      </c>
-    </row>
-    <row r="232" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A232">
-        <v>13.625</v>
-      </c>
-      <c r="B232">
-        <v>3.7083333000000001</v>
-      </c>
-      <c r="C232">
-        <v>5.1666664999999998</v>
-      </c>
-    </row>
-    <row r="233" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A233">
-        <v>1.4059139</v>
-      </c>
-      <c r="B233">
-        <v>1.3413979</v>
-      </c>
-      <c r="C233">
-        <v>13.303763</v>
-      </c>
-    </row>
-    <row r="234" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A234">
-        <v>8.75</v>
-      </c>
-      <c r="B234">
-        <v>13</v>
-      </c>
-      <c r="C234">
-        <v>13.75</v>
-      </c>
-    </row>
-    <row r="235" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A235">
-        <v>6.4545455</v>
-      </c>
-      <c r="B235">
-        <v>3.5</v>
-      </c>
-      <c r="C235">
-        <v>0.84090905999999999</v>
-      </c>
-    </row>
-    <row r="236" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A236">
-        <v>3.5707548</v>
-      </c>
-      <c r="B236">
-        <v>8.7169808999999994</v>
-      </c>
-      <c r="C236">
-        <v>3.7028300999999999</v>
-      </c>
-    </row>
-    <row r="237" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A237">
-        <v>13.544117999999999</v>
-      </c>
-      <c r="B237">
-        <v>3.6911763999999998</v>
-      </c>
-      <c r="C237">
-        <v>8.5147057000000004</v>
-      </c>
-    </row>
-    <row r="238" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A238">
-        <v>10.558332999999999</v>
-      </c>
-      <c r="B238">
-        <v>4.8249997999999996</v>
-      </c>
-      <c r="C238">
-        <v>6.6500000999999997</v>
-      </c>
-    </row>
-    <row r="239" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A239">
-        <v>13.201219999999999</v>
-      </c>
-      <c r="B239">
-        <v>0.84756100000000001</v>
-      </c>
-      <c r="C239">
-        <v>1.6280488</v>
-      </c>
-    </row>
-    <row r="240" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A240">
-        <v>6.2874999000000003</v>
-      </c>
-      <c r="B240">
-        <v>12.887499999999999</v>
-      </c>
-      <c r="C240">
-        <v>2.9708332999999998</v>
-      </c>
-    </row>
-    <row r="241" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A241">
-        <v>13.108025</v>
-      </c>
-      <c r="B241">
-        <v>7.5709876999999999</v>
-      </c>
-      <c r="C241">
-        <v>2.6697530999999999</v>
-      </c>
-    </row>
-    <row r="242" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A242">
-        <v>0.64999998000000003</v>
-      </c>
-      <c r="B242">
-        <v>13.55</v>
-      </c>
-      <c r="C242">
-        <v>13.5</v>
-      </c>
-    </row>
-    <row r="243" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A243">
-        <v>4.9780702999999997</v>
-      </c>
-      <c r="B243">
-        <v>3.8552632</v>
-      </c>
-      <c r="C243">
-        <v>9.8815793999999997</v>
-      </c>
-    </row>
-    <row r="244" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A244">
-        <v>7.8131069999999996</v>
-      </c>
-      <c r="B244">
-        <v>10.691748</v>
-      </c>
-      <c r="C244">
-        <v>1.1286408000000001</v>
-      </c>
-    </row>
-    <row r="245" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A245">
-        <v>8.8284310999999995</v>
-      </c>
-      <c r="B245">
-        <v>10.936275</v>
-      </c>
-      <c r="C245">
-        <v>5.2107843999999996</v>
-      </c>
-    </row>
-    <row r="246" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A246">
-        <v>10.726744999999999</v>
-      </c>
-      <c r="B246">
-        <v>12.093023000000001</v>
-      </c>
-      <c r="C246">
-        <v>2.9767442000000002</v>
-      </c>
-    </row>
-    <row r="247" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A247">
-        <v>1.1722223000000001</v>
-      </c>
-      <c r="B247">
-        <v>7.0611110000000004</v>
-      </c>
-      <c r="C247">
-        <v>10.438889</v>
-      </c>
-    </row>
-    <row r="248" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A248">
-        <v>6.5637255000000003</v>
-      </c>
-      <c r="B248">
-        <v>12.828431</v>
-      </c>
-      <c r="C248">
-        <v>0.92647058000000004</v>
-      </c>
-    </row>
-    <row r="249" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A249">
-        <v>4.6691918000000001</v>
-      </c>
-      <c r="B249">
-        <v>3.7904040999999999</v>
-      </c>
-      <c r="C249">
-        <v>13.270201999999999</v>
-      </c>
-    </row>
-    <row r="250" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A250">
-        <v>11.863636</v>
-      </c>
-      <c r="B250">
-        <v>13.522727</v>
-      </c>
-      <c r="C250">
-        <v>4.2045455</v>
-      </c>
-    </row>
-    <row r="251" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A251">
-        <v>11.304688000000001</v>
-      </c>
-      <c r="B251">
-        <v>8.4765625</v>
-      </c>
-      <c r="C251">
-        <v>5.9140625</v>
-      </c>
-    </row>
-    <row r="252" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A252">
-        <v>0.92424244</v>
-      </c>
-      <c r="B252">
-        <v>5.4318179999999998</v>
-      </c>
-      <c r="C252">
-        <v>0.73484850000000002</v>
-      </c>
-    </row>
-    <row r="253" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A253">
-        <v>3.048969</v>
-      </c>
-      <c r="B253">
-        <v>2.6829896</v>
-      </c>
-      <c r="C253">
-        <v>10.136597999999999</v>
-      </c>
-    </row>
-    <row r="254" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A254">
-        <v>2</v>
-      </c>
-      <c r="B254">
-        <v>4.3375000999999997</v>
-      </c>
-      <c r="C254">
-        <v>6.9562502000000004</v>
+        <v>3.8273809000000001</v>
       </c>
     </row>
   </sheetData>
@@ -4045,21 +3066,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100CAC4D93A0575064389BD540435903E82" ma:contentTypeVersion="10" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="66321db909bf898dba8428bb42a2284f">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="fafecb2a-7d6f-4b9a-8121-3bd755021f65" xmlns:ns4="66ca9c6c-5ec7-4bb0-a402-09c5f6e4f3bb" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="2a4762e9ded194d4c2e552f68b1d406a" ns3:_="" ns4:_="">
     <xsd:import namespace="fafecb2a-7d6f-4b9a-8121-3bd755021f65"/>
@@ -4262,24 +3268,22 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3BF7FACE-1743-4185-A432-BBDBC75AE110}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{84B75DF6-E9B7-46AF-A237-716DDC59A331}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4EABAF8D-4883-43A9-AA73-56294289EE7E}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -4296,4 +3300,29 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3BF7FACE-1743-4185-A432-BBDBC75AE110}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{84B75DF6-E9B7-46AF-A237-716DDC59A331}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="66ca9c6c-5ec7-4bb0-a402-09c5f6e4f3bb"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="fafecb2a-7d6f-4b9a-8121-3bd755021f65"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>